<commit_message>
tc changes from tc45 - 61
Signed-off-by: Akul <abhutani@navatargroup.com>
</commit_message>
<xml_diff>
--- a/SmokeTestCases.xlsx
+++ b/SmokeTestCases.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="19"/>
   </bookViews>
   <sheets>
     <sheet name="Institutions" sheetId="1" state="visible" r:id="rId2"/>
@@ -38,45 +38,8 @@
 </workbook>
 </file>
 
-<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
-  <authors>
-    <author> </author>
-  </authors>
-  <commentList>
-    <comment ref="C6" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b val="true"/>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">Author:
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">Create these contacts only from Contacts related list available at Institutions.
-Mailling and Others address needs to be populated from Account page.</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="892" uniqueCount="524">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="893" uniqueCount="524">
   <si>
     <t xml:space="preserve">Variable_Name</t>
   </si>
@@ -426,7 +389,7 @@
     <t xml:space="preserve">SmokeFRC1</t>
   </si>
   <si>
-    <t xml:space="preserve">FC - 146</t>
+    <t xml:space="preserve">FC - 149</t>
   </si>
   <si>
     <t xml:space="preserve">TestM1Institution1 - TestM1Fund1</t>
@@ -447,7 +410,7 @@
     <t xml:space="preserve">SmokeFRC3</t>
   </si>
   <si>
-    <t xml:space="preserve">FC - 147</t>
+    <t xml:space="preserve">FC - 150</t>
   </si>
   <si>
     <t xml:space="preserve">TestM1Institution2 - TestM1Fund1</t>
@@ -462,7 +425,7 @@
     <t xml:space="preserve">SmokeFRC4</t>
   </si>
   <si>
-    <t xml:space="preserve">FC - 148</t>
+    <t xml:space="preserve">FC - 151</t>
   </si>
   <si>
     <t xml:space="preserve">M1Contact4</t>
@@ -471,7 +434,7 @@
     <t xml:space="preserve">SmokeFRC5</t>
   </si>
   <si>
-    <t xml:space="preserve">FC - 149</t>
+    <t xml:space="preserve">FC - 152</t>
   </si>
   <si>
     <t xml:space="preserve">TestM1Institution2 - TestM1Fund2</t>
@@ -480,13 +443,13 @@
     <t xml:space="preserve">SmokeFRC6</t>
   </si>
   <si>
-    <t xml:space="preserve">FC - 150</t>
+    <t xml:space="preserve">FC - 153</t>
   </si>
   <si>
     <t xml:space="preserve">SmokeFRC7</t>
   </si>
   <si>
-    <t xml:space="preserve">FC - 151</t>
+    <t xml:space="preserve">FC - 154</t>
   </si>
   <si>
     <t xml:space="preserve">TestM1Institution1 - TestM1Fund3</t>
@@ -495,7 +458,7 @@
     <t xml:space="preserve">SmokeFRC8</t>
   </si>
   <si>
-    <t xml:space="preserve">FC - 152</t>
+    <t xml:space="preserve">FC - 155</t>
   </si>
   <si>
     <t xml:space="preserve">TestM1Institution2 - TestM1Fund3</t>
@@ -504,7 +467,7 @@
     <t xml:space="preserve">SmokeFRC9</t>
   </si>
   <si>
-    <t xml:space="preserve">FC - 153</t>
+    <t xml:space="preserve">FC - 156</t>
   </si>
   <si>
     <t xml:space="preserve">Contact_EmailId</t>
@@ -558,7 +521,7 @@
     <t xml:space="preserve">SmokeC1</t>
   </si>
   <si>
-    <t xml:space="preserve">deelroom+79864@gmail.com</t>
+    <t xml:space="preserve">deelroom+69569@gmail.com</t>
   </si>
   <si>
     <t xml:space="preserve">SmokeC2</t>
@@ -567,13 +530,13 @@
     <t xml:space="preserve">M1Contact2</t>
   </si>
   <si>
-    <t xml:space="preserve">deelroom+41020@gmail.com</t>
+    <t xml:space="preserve">deelroom+94693@gmail.com</t>
   </si>
   <si>
     <t xml:space="preserve">SmokeC3</t>
   </si>
   <si>
-    <t xml:space="preserve">deelroom+15819@gmail.com</t>
+    <t xml:space="preserve">deelroom+25891@gmail.com</t>
   </si>
   <si>
     <t xml:space="preserve">SmokeC4</t>
@@ -585,7 +548,7 @@
     <t xml:space="preserve">Mike</t>
   </si>
   <si>
-    <t xml:space="preserve">deelroom+16569@gmail.com</t>
+    <t xml:space="preserve">deelroom+71019@gmail.com</t>
   </si>
   <si>
     <t xml:space="preserve">SmokeC6</t>
@@ -597,7 +560,7 @@
     <t xml:space="preserve">Reddick</t>
   </si>
   <si>
-    <t xml:space="preserve">deelroom+91676@gmail.com</t>
+    <t xml:space="preserve">deelroom+91215@gmail.com</t>
   </si>
   <si>
     <t xml:space="preserve">Botanical Garden</t>
@@ -615,7 +578,7 @@
     <t xml:space="preserve">Wick</t>
   </si>
   <si>
-    <t xml:space="preserve">deelroom+74427@gmail.com</t>
+    <t xml:space="preserve">deelroom+90837@gmail.com</t>
   </si>
   <si>
     <t xml:space="preserve">Robert</t>
@@ -636,7 +599,7 @@
     <t xml:space="preserve">Smith</t>
   </si>
   <si>
-    <t xml:space="preserve">deelroom+49521@gmail.com</t>
+    <t xml:space="preserve">deelroom+55391@gmail.com</t>
   </si>
   <si>
     <t xml:space="preserve">Julie</t>
@@ -675,10 +638,10 @@
     <t xml:space="preserve">Fund</t>
   </si>
   <si>
-    <t xml:space="preserve">3.75E8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10/14/2019</t>
+    <t xml:space="preserve">4.5E8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7/02/2020</t>
   </si>
   <si>
     <t xml:space="preserve">SmokeFund2</t>
@@ -696,7 +659,7 @@
     <t xml:space="preserve">TestM1Fund3</t>
   </si>
   <si>
-    <t xml:space="preserve">2.8E7</t>
+    <t xml:space="preserve">4.2E7</t>
   </si>
   <si>
     <t xml:space="preserve">Fundraising_Name</t>
@@ -801,7 +764,7 @@
     <t xml:space="preserve">SmokePL1</t>
   </si>
   <si>
-    <t xml:space="preserve">TestCompany1 - Mar 2020</t>
+    <t xml:space="preserve">TestCompany1 - Jul 2020</t>
   </si>
   <si>
     <t xml:space="preserve">TestCompany1</t>
@@ -810,9 +773,6 @@
     <t xml:space="preserve">Today's date</t>
   </si>
   <si>
-    <t xml:space="preserve">Idea Generation</t>
-  </si>
-  <si>
     <t xml:space="preserve">Listing Agreement</t>
   </si>
   <si>
@@ -825,13 +785,13 @@
     <t xml:space="preserve">New/Initial Interest</t>
   </si>
   <si>
-    <t xml:space="preserve">Declined/Dead</t>
+    <t xml:space="preserve">Declined</t>
   </si>
   <si>
     <t xml:space="preserve">SmokePL2</t>
   </si>
   <si>
-    <t xml:space="preserve">TestCompany2 - Mar 2020</t>
+    <t xml:space="preserve">TestCompany2 - Jul 2020</t>
   </si>
   <si>
     <t xml:space="preserve">TestCompany2</t>
@@ -858,7 +818,7 @@
     <t xml:space="preserve">SmokePL3</t>
   </si>
   <si>
-    <t xml:space="preserve">TestCompany3 - Mar 2020</t>
+    <t xml:space="preserve">TestCompany3 - Jul 2020</t>
   </si>
   <si>
     <t xml:space="preserve">TestCompany3</t>
@@ -1005,7 +965,7 @@
     <t xml:space="preserve">SmokeCOMM1</t>
   </si>
   <si>
-    <t xml:space="preserve">CMT - 000930</t>
+    <t xml:space="preserve">CMT - 000936</t>
   </si>
   <si>
     <t xml:space="preserve">LP</t>
@@ -1014,61 +974,61 @@
     <t xml:space="preserve">W-9</t>
   </si>
   <si>
-    <t xml:space="preserve">3/18/2020</t>
+    <t xml:space="preserve">7/2/2020</t>
   </si>
   <si>
     <t xml:space="preserve">SmokeCOMM2</t>
   </si>
   <si>
-    <t xml:space="preserve">CMT - 000931</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3/20/2020</t>
+    <t xml:space="preserve">CMT - 000937</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7/3/2020</t>
   </si>
   <si>
     <t xml:space="preserve">SmokeCOMM3</t>
   </si>
   <si>
-    <t xml:space="preserve">CMT - 000932</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3/22/2020</t>
+    <t xml:space="preserve">CMT - 000938</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7/5/2020</t>
   </si>
   <si>
     <t xml:space="preserve">SmokeCOMM4</t>
   </si>
   <si>
-    <t xml:space="preserve">CMT - 000933</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3/23/2020</t>
+    <t xml:space="preserve">CMT - 000939</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7/6/2020</t>
   </si>
   <si>
     <t xml:space="preserve">SmokeCOMM5</t>
   </si>
   <si>
-    <t xml:space="preserve">CMT - 000934</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3/26/2020</t>
+    <t xml:space="preserve">CMT - 000940</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7/9/2020</t>
   </si>
   <si>
     <t xml:space="preserve">SmokeCOMM6</t>
   </si>
   <si>
-    <t xml:space="preserve">CMT - 000935</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3/29/2020</t>
+    <t xml:space="preserve">CMT - 000941</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7/12/2020</t>
   </si>
   <si>
     <t xml:space="preserve">SmokeCOMM7</t>
   </si>
   <si>
-    <t xml:space="preserve">CMT - 000936</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4/3/2020</t>
+    <t xml:space="preserve">CMT - 000942</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7/17/2020</t>
   </si>
   <si>
     <t xml:space="preserve">SmokeCOMM8</t>
@@ -1134,10 +1094,10 @@
     <t xml:space="preserve">CC1</t>
   </si>
   <si>
-    <t xml:space="preserve">CC-0619</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DD-0215</t>
+    <t xml:space="preserve">CC-0621</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DD-0214</t>
   </si>
   <si>
     <t xml:space="preserve">250000</t>
@@ -1146,7 +1106,7 @@
     <t xml:space="preserve">2500000</t>
   </si>
   <si>
-    <t xml:space="preserve">3/19/2020</t>
+    <t xml:space="preserve">7/7/2020</t>
   </si>
   <si>
     <t xml:space="preserve">3/26/2019</t>
@@ -1158,7 +1118,7 @@
     <t xml:space="preserve">CC2</t>
   </si>
   <si>
-    <t xml:space="preserve">CC-0620</t>
+    <t xml:space="preserve">CC-0622</t>
   </si>
   <si>
     <t xml:space="preserve">400000</t>
@@ -1179,7 +1139,7 @@
     <t xml:space="preserve">CC3</t>
   </si>
   <si>
-    <t xml:space="preserve">CC-0621</t>
+    <t xml:space="preserve">CC-0623</t>
   </si>
   <si>
     <t xml:space="preserve">1600000</t>
@@ -1194,7 +1154,7 @@
     <t xml:space="preserve">CC4</t>
   </si>
   <si>
-    <t xml:space="preserve">CC-0622</t>
+    <t xml:space="preserve">CC-0624</t>
   </si>
   <si>
     <t xml:space="preserve">1200000</t>
@@ -1215,7 +1175,7 @@
     <t xml:space="preserve">CC5</t>
   </si>
   <si>
-    <t xml:space="preserve">CC-0623</t>
+    <t xml:space="preserve">CC-0625</t>
   </si>
   <si>
     <t xml:space="preserve">800000</t>
@@ -1278,7 +1238,7 @@
     <t xml:space="preserve">FD1</t>
   </si>
   <si>
-    <t xml:space="preserve">FD-0228</t>
+    <t xml:space="preserve">FD-0226</t>
   </si>
   <si>
     <t xml:space="preserve">InvestorDistributionID</t>
@@ -1287,7 +1247,7 @@
     <t xml:space="preserve">ID1</t>
   </si>
   <si>
-    <t xml:space="preserve">ID-0625</t>
+    <t xml:space="preserve">ID-0627</t>
   </si>
   <si>
     <t xml:space="preserve">25000000</t>
@@ -1305,7 +1265,7 @@
     <t xml:space="preserve">ID2</t>
   </si>
   <si>
-    <t xml:space="preserve">ID-0626</t>
+    <t xml:space="preserve">ID-0628</t>
   </si>
   <si>
     <t xml:space="preserve">66666.667</t>
@@ -1317,7 +1277,7 @@
     <t xml:space="preserve">ID3</t>
   </si>
   <si>
-    <t xml:space="preserve">ID-0627</t>
+    <t xml:space="preserve">ID-0629</t>
   </si>
   <si>
     <t xml:space="preserve">266666.667</t>
@@ -1326,7 +1286,7 @@
     <t xml:space="preserve">ID4</t>
   </si>
   <si>
-    <t xml:space="preserve">ID-0628</t>
+    <t xml:space="preserve">ID-0630</t>
   </si>
   <si>
     <t xml:space="preserve">15000000</t>
@@ -1344,10 +1304,7 @@
     <t xml:space="preserve">ID5</t>
   </si>
   <si>
-    <t xml:space="preserve">FD-0248</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ID-0629</t>
+    <t xml:space="preserve">ID-0631</t>
   </si>
   <si>
     <t xml:space="preserve">133333.333</t>
@@ -1380,6 +1337,9 @@
     <t xml:space="preserve">Acct 2 Contact, Inst</t>
   </si>
   <si>
+    <t xml:space="preserve">7/4/2020</t>
+  </si>
+  <si>
     <t xml:space="preserve">Institution&lt;break&gt;ContactTransferAcc 1</t>
   </si>
   <si>
@@ -1443,13 +1403,13 @@
     <t xml:space="preserve">SuperAdmin</t>
   </si>
   <si>
-    <t xml:space="preserve">PE</t>
+    <t xml:space="preserve">PERE</t>
   </si>
   <si>
     <t xml:space="preserve">Admin</t>
   </si>
   <si>
-    <t xml:space="preserve">PE Standard User</t>
+    <t xml:space="preserve">PE Real Estate</t>
   </si>
   <si>
     <t xml:space="preserve">Salesforce Platform</t>
@@ -1461,7 +1421,10 @@
     <t xml:space="preserve">CRMUser1</t>
   </si>
   <si>
-    <t xml:space="preserve">User</t>
+    <t xml:space="preserve">User28335</t>
+  </si>
+  <si>
+    <t xml:space="preserve">automationnavatar+61008@gmail.com</t>
   </si>
   <si>
     <t xml:space="preserve">Nick</t>
@@ -1663,7 +1626,7 @@
     <numFmt numFmtId="169" formatCode="\$#,##0.00_);[RED]&quot;($&quot;#,##0.00\)"/>
     <numFmt numFmtId="170" formatCode="[$-409]M/D/YYYY"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1699,21 +1662,6 @@
       <sz val="11"/>
       <color rgb="FF0563C1"/>
       <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="9"/>
-      <color rgb="FF000000"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color rgb="FF000000"/>
-      <name val="Tahoma"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
@@ -1987,7 +1935,7 @@
   </sheetPr>
   <dimension ref="A1:W15"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="C16" activeCellId="0" sqref="C16"/>
@@ -2010,11 +1958,11 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="11.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="8.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="15.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="8.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="8.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="15.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="13.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="19.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="20" style="0" width="17.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="20" style="0" width="17.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="10.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="10"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="24" style="0" width="8.67"/>
@@ -2514,21 +2462,21 @@
         <v>0</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C1" s="9" t="s">
         <v>189</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
+        <v>280</v>
+      </c>
+      <c r="B2" s="0" t="s">
         <v>281</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>282</v>
       </c>
       <c r="C2" s="0" t="s">
         <v>197</v>
@@ -2536,24 +2484,24 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
+        <v>282</v>
+      </c>
+      <c r="B3" s="0" t="s">
         <v>283</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>284</v>
       </c>
       <c r="C3" s="0" t="s">
         <v>197</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
+        <v>285</v>
+      </c>
+      <c r="B4" s="0" t="s">
         <v>286</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>287</v>
       </c>
       <c r="C4" s="0" t="s">
         <v>205</v>
@@ -2561,10 +2509,10 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
+        <v>287</v>
+      </c>
+      <c r="B5" s="0" t="s">
         <v>288</v>
-      </c>
-      <c r="B5" s="0" t="s">
-        <v>289</v>
       </c>
       <c r="C5" s="0" t="s">
         <v>205</v>
@@ -2598,7 +2546,7 @@
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="23.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="23.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="25.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="23.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="13.29"/>
@@ -2606,14 +2554,14 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="22.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="16.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="18.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="2" width="19.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="2" width="19.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="2" width="22.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="2" width="21.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="2" width="22.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="22.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="13.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="21.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="35.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="35.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="33.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="16.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="21" style="0" width="8.67"/>
@@ -2624,87 +2572,87 @@
         <v>0</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C1" s="9" t="s">
         <v>90</v>
       </c>
       <c r="D1" s="9" t="s">
+        <v>290</v>
+      </c>
+      <c r="E1" s="9" t="s">
         <v>291</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="F1" s="9" t="s">
         <v>292</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="G1" s="9" t="s">
         <v>293</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="H1" s="9" t="s">
         <v>294</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="I1" s="9" t="s">
         <v>295</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="J1" s="9" t="s">
         <v>296</v>
       </c>
-      <c r="J1" s="9" t="s">
+      <c r="K1" s="18" t="s">
         <v>297</v>
       </c>
-      <c r="K1" s="18" t="s">
+      <c r="L1" s="18" t="s">
         <v>298</v>
       </c>
-      <c r="L1" s="18" t="s">
+      <c r="M1" s="18" t="s">
         <v>299</v>
       </c>
-      <c r="M1" s="18" t="s">
+      <c r="N1" s="18" t="s">
         <v>300</v>
       </c>
-      <c r="N1" s="18" t="s">
+      <c r="O1" s="9" t="s">
         <v>301</v>
       </c>
-      <c r="O1" s="9" t="s">
+      <c r="P1" s="9" t="s">
         <v>302</v>
       </c>
-      <c r="P1" s="9" t="s">
+      <c r="Q1" s="19" t="s">
         <v>303</v>
       </c>
-      <c r="Q1" s="19" t="s">
+      <c r="R1" s="20" t="s">
         <v>304</v>
       </c>
-      <c r="R1" s="20" t="s">
+      <c r="S1" s="19" t="s">
         <v>305</v>
       </c>
-      <c r="S1" s="19" t="s">
+      <c r="T1" s="9" t="s">
         <v>306</v>
-      </c>
-      <c r="T1" s="9" t="s">
-        <v>307</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
+        <v>307</v>
+      </c>
+      <c r="B2" s="0" t="s">
         <v>308</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>309</v>
       </c>
       <c r="C2" s="0" t="s">
         <v>94</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="E2" s="0" t="n">
         <v>20000000</v>
       </c>
       <c r="F2" s="0" t="s">
+        <v>309</v>
+      </c>
+      <c r="G2" s="0" t="s">
         <v>310</v>
       </c>
-      <c r="G2" s="0" t="s">
+      <c r="H2" s="0" t="s">
         <v>311</v>
-      </c>
-      <c r="H2" s="0" t="s">
-        <v>312</v>
       </c>
       <c r="P2" s="21"/>
       <c r="T2" s="22" t="s">
@@ -2713,49 +2661,49 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
+        <v>312</v>
+      </c>
+      <c r="B3" s="0" t="s">
         <v>313</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>314</v>
       </c>
       <c r="C3" s="0" t="s">
         <v>99</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="E3" s="0" t="n">
         <v>10000000</v>
       </c>
       <c r="F3" s="0" t="s">
+        <v>309</v>
+      </c>
+      <c r="G3" s="0" t="s">
         <v>310</v>
       </c>
-      <c r="G3" s="0" t="s">
-        <v>311</v>
-      </c>
       <c r="H3" s="0" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="T3" s="22"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
+        <v>315</v>
+      </c>
+      <c r="B4" s="0" t="s">
         <v>316</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>317</v>
       </c>
       <c r="C4" s="0" t="s">
         <v>94</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="E4" s="0" t="n">
         <v>15000000</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="J4" s="0" t="n">
         <v>7.5</v>
@@ -2764,22 +2712,22 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
+        <v>318</v>
+      </c>
+      <c r="B5" s="0" t="s">
         <v>319</v>
-      </c>
-      <c r="B5" s="0" t="s">
-        <v>320</v>
       </c>
       <c r="C5" s="0" t="s">
         <v>102</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="E5" s="0" t="n">
         <v>25000000</v>
       </c>
       <c r="H5" s="0" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="J5" s="0" t="n">
         <v>7.5</v>
@@ -2788,43 +2736,43 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
+        <v>321</v>
+      </c>
+      <c r="B6" s="0" t="s">
         <v>322</v>
-      </c>
-      <c r="B6" s="0" t="s">
-        <v>323</v>
       </c>
       <c r="C6" s="0" t="s">
         <v>105</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="E6" s="0" t="n">
         <v>5000000</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="T6" s="22"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
+        <v>324</v>
+      </c>
+      <c r="B7" s="0" t="s">
         <v>325</v>
-      </c>
-      <c r="B7" s="0" t="s">
-        <v>326</v>
       </c>
       <c r="C7" s="0" t="s">
         <v>105</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="E7" s="0" t="n">
         <v>2000000</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="I7" s="0" t="s">
         <v>52</v>
@@ -2833,22 +2781,22 @@
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
+        <v>327</v>
+      </c>
+      <c r="B8" s="0" t="s">
         <v>328</v>
-      </c>
-      <c r="B8" s="0" t="s">
-        <v>329</v>
       </c>
       <c r="C8" s="0" t="s">
         <v>107</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="E8" s="0" t="n">
         <v>12000000</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="I8" s="0" t="s">
         <v>52</v>
@@ -2857,31 +2805,31 @@
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C9" s="0" t="s">
         <v>94</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="E9" s="0" t="n">
         <v>20000000</v>
       </c>
       <c r="F9" s="0" t="s">
+        <v>309</v>
+      </c>
+      <c r="G9" s="0" t="s">
         <v>310</v>
       </c>
-      <c r="G9" s="0" t="s">
+      <c r="H9" s="0" t="s">
         <v>311</v>
       </c>
-      <c r="H9" s="0" t="s">
-        <v>312</v>
-      </c>
       <c r="K9" s="2" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="L9" s="2" t="n">
         <v>2000000</v>
@@ -2893,45 +2841,45 @@
         <v>0</v>
       </c>
       <c r="O9" s="2" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="P9" s="2" t="n">
         <v>0</v>
       </c>
       <c r="Q9" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="R9" s="2" t="s">
         <v>334</v>
-      </c>
-      <c r="R9" s="2" t="s">
-        <v>335</v>
       </c>
       <c r="S9" s="0" t="n">
         <v>0</v>
       </c>
       <c r="T9" s="0" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
+        <v>336</v>
+      </c>
+      <c r="B10" s="0" t="s">
         <v>337</v>
-      </c>
-      <c r="B10" s="0" t="s">
-        <v>338</v>
       </c>
       <c r="C10" s="0" t="s">
         <v>94</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="E10" s="0" t="n">
         <v>20000000</v>
       </c>
       <c r="F10" s="0" t="s">
+        <v>309</v>
+      </c>
+      <c r="G10" s="0" t="s">
         <v>310</v>
-      </c>
-      <c r="G10" s="0" t="s">
-        <v>311</v>
       </c>
       <c r="H10" s="0" t="s">
         <v>243</v>
@@ -2949,7 +2897,7 @@
         <v>0</v>
       </c>
       <c r="O10" s="2" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="P10" s="2" t="n">
         <v>0</v>
@@ -2964,7 +2912,7 @@
         <v>0</v>
       </c>
       <c r="T10" s="0" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
   </sheetData>
@@ -3013,245 +2961,245 @@
         <v>0</v>
       </c>
       <c r="B1" s="18" t="s">
+        <v>339</v>
+      </c>
+      <c r="C1" s="9" t="s">
         <v>340</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="D1" s="18" t="s">
+        <v>289</v>
+      </c>
+      <c r="E1" s="18" t="s">
         <v>341</v>
       </c>
-      <c r="D1" s="18" t="s">
-        <v>290</v>
-      </c>
-      <c r="E1" s="18" t="s">
+      <c r="F1" s="18" t="s">
         <v>342</v>
       </c>
-      <c r="F1" s="18" t="s">
+      <c r="G1" s="18" t="s">
         <v>343</v>
       </c>
-      <c r="G1" s="18" t="s">
+      <c r="H1" s="18" t="s">
         <v>344</v>
       </c>
-      <c r="H1" s="18" t="s">
+      <c r="I1" s="18" t="s">
         <v>345</v>
       </c>
-      <c r="I1" s="18" t="s">
+      <c r="J1" s="18" t="s">
         <v>346</v>
       </c>
-      <c r="J1" s="18" t="s">
+      <c r="K1" s="18" t="s">
         <v>347</v>
       </c>
-      <c r="K1" s="18" t="s">
+      <c r="L1" s="18" t="s">
         <v>348</v>
       </c>
-      <c r="L1" s="18" t="s">
+      <c r="M1" s="18" t="s">
         <v>349</v>
-      </c>
-      <c r="M1" s="18" t="s">
-        <v>350</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
+        <v>350</v>
+      </c>
+      <c r="B2" s="0" t="s">
         <v>351</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="C2" s="0" t="s">
         <v>352</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="D2" s="0" t="s">
+        <v>319</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>331</v>
+      </c>
+      <c r="F2" s="0" t="s">
         <v>353</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="G2" s="0" t="s">
+        <v>353</v>
+      </c>
+      <c r="H2" s="0" t="s">
+        <v>354</v>
+      </c>
+      <c r="I2" s="0" t="s">
         <v>320</v>
       </c>
-      <c r="E2" s="0" t="s">
-        <v>332</v>
-      </c>
-      <c r="F2" s="0" t="s">
-        <v>354</v>
-      </c>
-      <c r="G2" s="0" t="s">
-        <v>354</v>
-      </c>
-      <c r="H2" s="0" t="s">
+      <c r="J2" s="0" t="s">
         <v>355</v>
       </c>
-      <c r="I2" s="0" t="s">
+      <c r="K2" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="L2" s="25" t="s">
         <v>356</v>
       </c>
-      <c r="J2" s="0" t="s">
-        <v>315</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>332</v>
-      </c>
-      <c r="L2" s="25" t="s">
+      <c r="M2" s="0" t="s">
         <v>357</v>
-      </c>
-      <c r="M2" s="0" t="s">
-        <v>358</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="B3" s="0" t="s">
         <v>359</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="C3" s="0" t="s">
+        <v>352</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>322</v>
+      </c>
+      <c r="E3" s="0" t="s">
         <v>360</v>
       </c>
-      <c r="C3" s="0" t="s">
-        <v>353</v>
-      </c>
-      <c r="D3" s="0" t="s">
-        <v>323</v>
-      </c>
-      <c r="E3" s="0" t="s">
+      <c r="F3" s="0" t="s">
         <v>361</v>
       </c>
-      <c r="F3" s="0" t="s">
+      <c r="G3" s="0" t="s">
+        <v>361</v>
+      </c>
+      <c r="H3" s="0" t="s">
         <v>362</v>
       </c>
-      <c r="G3" s="0" t="s">
-        <v>362</v>
-      </c>
-      <c r="H3" s="0" t="s">
-        <v>363</v>
-      </c>
       <c r="I3" s="0" t="s">
-        <v>356</v>
+        <v>320</v>
       </c>
       <c r="J3" s="0" t="s">
-        <v>315</v>
+        <v>355</v>
       </c>
       <c r="K3" s="2" t="s">
         <v>95</v>
       </c>
       <c r="L3" s="2" t="s">
+        <v>363</v>
+      </c>
+      <c r="M3" s="0" t="s">
         <v>364</v>
-      </c>
-      <c r="M3" s="0" t="s">
-        <v>365</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
+        <v>365</v>
+      </c>
+      <c r="B4" s="0" t="s">
         <v>366</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="C4" s="0" t="s">
+        <v>352</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>308</v>
+      </c>
+      <c r="E4" s="0" t="s">
         <v>367</v>
       </c>
-      <c r="C4" s="0" t="s">
-        <v>353</v>
-      </c>
-      <c r="D4" s="0" t="s">
-        <v>309</v>
-      </c>
-      <c r="E4" s="0" t="s">
+      <c r="F4" s="0" t="s">
         <v>368</v>
       </c>
-      <c r="F4" s="0" t="s">
+      <c r="G4" s="0" t="s">
+        <v>368</v>
+      </c>
+      <c r="H4" s="0" t="s">
+        <v>331</v>
+      </c>
+      <c r="I4" s="0" t="s">
+        <v>320</v>
+      </c>
+      <c r="J4" s="0" t="s">
+        <v>355</v>
+      </c>
+      <c r="K4" s="0" t="s">
+        <v>331</v>
+      </c>
+      <c r="L4" s="0" t="s">
+        <v>320</v>
+      </c>
+      <c r="M4" s="0" t="s">
         <v>369</v>
-      </c>
-      <c r="G4" s="0" t="s">
-        <v>369</v>
-      </c>
-      <c r="H4" s="0" t="s">
-        <v>332</v>
-      </c>
-      <c r="I4" s="0" t="s">
-        <v>356</v>
-      </c>
-      <c r="J4" s="0" t="s">
-        <v>315</v>
-      </c>
-      <c r="K4" s="0" t="s">
-        <v>332</v>
-      </c>
-      <c r="L4" s="0" t="s">
-        <v>356</v>
-      </c>
-      <c r="M4" s="0" t="s">
-        <v>370</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
+        <v>370</v>
+      </c>
+      <c r="B5" s="0" t="s">
         <v>371</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="C5" s="0" t="s">
+        <v>352</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>316</v>
+      </c>
+      <c r="E5" s="0" t="s">
         <v>372</v>
       </c>
-      <c r="C5" s="0" t="s">
-        <v>353</v>
-      </c>
-      <c r="D5" s="0" t="s">
-        <v>317</v>
-      </c>
-      <c r="E5" s="0" t="s">
+      <c r="F5" s="0" t="s">
         <v>373</v>
       </c>
-      <c r="F5" s="0" t="s">
+      <c r="G5" s="0" t="s">
+        <v>373</v>
+      </c>
+      <c r="H5" s="0" t="s">
         <v>374</v>
       </c>
-      <c r="G5" s="0" t="s">
-        <v>374</v>
-      </c>
-      <c r="H5" s="0" t="s">
-        <v>375</v>
-      </c>
       <c r="I5" s="0" t="s">
-        <v>356</v>
+        <v>320</v>
       </c>
       <c r="J5" s="0" t="s">
-        <v>315</v>
+        <v>355</v>
       </c>
       <c r="K5" s="2" t="s">
         <v>95</v>
       </c>
       <c r="L5" s="2" t="s">
+        <v>375</v>
+      </c>
+      <c r="M5" s="0" t="s">
         <v>376</v>
-      </c>
-      <c r="M5" s="0" t="s">
-        <v>377</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="B6" s="0" t="s">
         <v>378</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="C6" s="0" t="s">
+        <v>352</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>313</v>
+      </c>
+      <c r="E6" s="0" t="s">
         <v>379</v>
       </c>
-      <c r="C6" s="0" t="s">
-        <v>353</v>
-      </c>
-      <c r="D6" s="0" t="s">
-        <v>314</v>
-      </c>
-      <c r="E6" s="0" t="s">
+      <c r="F6" s="0" t="s">
         <v>380</v>
       </c>
-      <c r="F6" s="0" t="s">
+      <c r="G6" s="0" t="s">
+        <v>380</v>
+      </c>
+      <c r="H6" s="0" t="s">
         <v>381</v>
       </c>
-      <c r="G6" s="0" t="s">
-        <v>381</v>
-      </c>
-      <c r="H6" s="0" t="s">
-        <v>382</v>
-      </c>
       <c r="I6" s="0" t="s">
-        <v>356</v>
+        <v>320</v>
       </c>
       <c r="J6" s="0" t="s">
-        <v>315</v>
+        <v>355</v>
       </c>
       <c r="K6" s="2" t="s">
         <v>95</v>
       </c>
       <c r="L6" s="2" t="s">
+        <v>382</v>
+      </c>
+      <c r="M6" s="0" t="s">
         <v>383</v>
-      </c>
-      <c r="M6" s="0" t="s">
-        <v>384</v>
       </c>
     </row>
   </sheetData>
@@ -3288,7 +3236,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="14.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="8.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="9.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="19.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="19.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="23.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="19.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="15" style="0" width="8.67"/>
@@ -3299,66 +3247,66 @@
         <v>0</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="C1" s="9" t="s">
         <v>189</v>
       </c>
       <c r="D1" s="9" t="s">
+        <v>344</v>
+      </c>
+      <c r="E1" s="9" t="s">
         <v>345</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="F1" s="9" t="s">
         <v>346</v>
       </c>
-      <c r="F1" s="9" t="s">
-        <v>347</v>
-      </c>
       <c r="G1" s="9" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="H1" s="9" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="I1" s="9" t="s">
+        <v>341</v>
+      </c>
+      <c r="J1" s="9" t="s">
         <v>342</v>
       </c>
-      <c r="J1" s="9" t="s">
+      <c r="K1" s="9" t="s">
         <v>343</v>
-      </c>
-      <c r="K1" s="9" t="s">
-        <v>344</v>
       </c>
       <c r="L1" s="9" t="s">
         <v>193</v>
       </c>
       <c r="M1" s="9" t="s">
+        <v>385</v>
+      </c>
+      <c r="N1" s="9" t="s">
         <v>386</v>
       </c>
-      <c r="N1" s="9" t="s">
+      <c r="O1" s="9" t="s">
         <v>387</v>
-      </c>
-      <c r="O1" s="9" t="s">
-        <v>388</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="C2" s="0" t="s">
         <v>197</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>356</v>
+        <v>320</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>315</v>
+        <v>355</v>
       </c>
       <c r="G2" s="2" t="n">
         <v>5500000</v>
@@ -3367,16 +3315,16 @@
         <v>2000000</v>
       </c>
       <c r="I2" s="2" t="s">
+        <v>390</v>
+      </c>
+      <c r="J2" s="2" t="s">
         <v>391</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>392</v>
       </c>
       <c r="K2" s="2" t="n">
         <v>750000</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="M2" s="2" t="n">
         <v>0</v>
@@ -3413,7 +3361,7 @@
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="11.71"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="11.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="8.67"/>
@@ -3428,48 +3376,48 @@
         <v>0</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="C1" s="9" t="s">
         <v>189</v>
       </c>
       <c r="D1" s="9" t="s">
+        <v>394</v>
+      </c>
+      <c r="E1" s="9" t="s">
         <v>395</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="F1" s="9" t="s">
+        <v>346</v>
+      </c>
+      <c r="G1" s="9" t="s">
         <v>396</v>
       </c>
-      <c r="F1" s="9" t="s">
-        <v>347</v>
-      </c>
-      <c r="G1" s="9" t="s">
+      <c r="H1" s="9" t="s">
+        <v>342</v>
+      </c>
+      <c r="I1" s="9" t="s">
         <v>397</v>
       </c>
-      <c r="H1" s="9" t="s">
-        <v>343</v>
-      </c>
-      <c r="I1" s="9" t="s">
-        <v>398</v>
-      </c>
       <c r="J1" s="9" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="K1" s="9" t="s">
+        <v>385</v>
+      </c>
+      <c r="L1" s="9" t="s">
         <v>386</v>
       </c>
-      <c r="L1" s="9" t="s">
+      <c r="M1" s="9" t="s">
         <v>387</v>
-      </c>
-      <c r="M1" s="9" t="s">
-        <v>388</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
+        <v>398</v>
+      </c>
+      <c r="B2" s="0" t="s">
         <v>399</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>400</v>
       </c>
       <c r="D2" s="0" t="n">
         <v>15000000</v>
@@ -3509,7 +3457,7 @@
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="3" style="0" width="20.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="13.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="8.67"/>
@@ -3524,200 +3472,200 @@
         <v>0</v>
       </c>
       <c r="B1" s="9" t="s">
+        <v>393</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>400</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>289</v>
+      </c>
+      <c r="E1" s="26" t="s">
+        <v>291</v>
+      </c>
+      <c r="F1" s="9" t="s">
         <v>394</v>
       </c>
-      <c r="C1" s="9" t="s">
-        <v>401</v>
-      </c>
-      <c r="D1" s="9" t="s">
-        <v>290</v>
-      </c>
-      <c r="E1" s="26" t="s">
-        <v>292</v>
-      </c>
-      <c r="F1" s="9" t="s">
+      <c r="G1" s="9" t="s">
         <v>395</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="H1" s="9" t="s">
         <v>396</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="I1" s="9" t="s">
         <v>397</v>
       </c>
-      <c r="I1" s="9" t="s">
-        <v>398</v>
-      </c>
       <c r="J1" s="9" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="M1" s="9" t="s">
+        <v>385</v>
+      </c>
+      <c r="N1" s="9" t="s">
         <v>386</v>
       </c>
-      <c r="N1" s="9" t="s">
+      <c r="O1" s="9" t="s">
         <v>387</v>
-      </c>
-      <c r="O1" s="9" t="s">
-        <v>388</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
+        <v>401</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>399</v>
+      </c>
+      <c r="C2" s="0" t="s">
         <v>402</v>
       </c>
-      <c r="B2" s="0" t="s">
-        <v>400</v>
-      </c>
-      <c r="C2" s="0" t="s">
+      <c r="D2" s="0" t="s">
+        <v>319</v>
+      </c>
+      <c r="E2" s="0" t="s">
         <v>403</v>
       </c>
-      <c r="D2" s="0" t="s">
-        <v>320</v>
-      </c>
-      <c r="E2" s="0" t="s">
+      <c r="F2" s="0" t="s">
         <v>404</v>
       </c>
-      <c r="F2" s="0" t="s">
+      <c r="G2" s="0" t="s">
         <v>405</v>
       </c>
-      <c r="G2" s="0" t="s">
+      <c r="H2" s="0" t="s">
+        <v>405</v>
+      </c>
+      <c r="I2" s="0" t="s">
+        <v>405</v>
+      </c>
+      <c r="J2" s="0" t="s">
         <v>406</v>
-      </c>
-      <c r="H2" s="0" t="s">
-        <v>406</v>
-      </c>
-      <c r="I2" s="0" t="s">
-        <v>406</v>
-      </c>
-      <c r="J2" s="0" t="s">
-        <v>407</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
+        <v>407</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>399</v>
+      </c>
+      <c r="C3" s="0" t="s">
         <v>408</v>
       </c>
-      <c r="B3" s="0" t="s">
-        <v>400</v>
-      </c>
-      <c r="C3" s="0" t="s">
+      <c r="D3" s="0" t="s">
+        <v>322</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>404</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>381</v>
+      </c>
+      <c r="G3" s="0" t="s">
         <v>409</v>
       </c>
-      <c r="D3" s="0" t="s">
-        <v>323</v>
-      </c>
-      <c r="E3" s="0" t="s">
-        <v>405</v>
-      </c>
-      <c r="F3" s="0" t="s">
-        <v>382</v>
-      </c>
-      <c r="G3" s="0" t="s">
+      <c r="H3" s="0" t="s">
+        <v>409</v>
+      </c>
+      <c r="I3" s="0" t="s">
+        <v>409</v>
+      </c>
+      <c r="J3" s="0" t="s">
         <v>410</v>
-      </c>
-      <c r="H3" s="0" t="s">
-        <v>410</v>
-      </c>
-      <c r="I3" s="0" t="s">
-        <v>410</v>
-      </c>
-      <c r="J3" s="0" t="s">
-        <v>411</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
+        <v>411</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>399</v>
+      </c>
+      <c r="C4" s="0" t="s">
         <v>412</v>
       </c>
-      <c r="B4" s="0" t="s">
-        <v>400</v>
-      </c>
-      <c r="C4" s="0" t="s">
-        <v>413</v>
-      </c>
       <c r="D4" s="0" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="E4" s="0" t="s">
         <v>96</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="I4" s="0" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="J4" s="0" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
+        <v>414</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>399</v>
+      </c>
+      <c r="C5" s="0" t="s">
         <v>415</v>
       </c>
-      <c r="B5" s="0" t="s">
-        <v>400</v>
-      </c>
-      <c r="C5" s="0" t="s">
+      <c r="D5" s="0" t="s">
+        <v>316</v>
+      </c>
+      <c r="E5" s="0" t="s">
         <v>416</v>
       </c>
-      <c r="D5" s="0" t="s">
-        <v>317</v>
-      </c>
-      <c r="E5" s="0" t="s">
+      <c r="F5" s="0" t="s">
         <v>417</v>
       </c>
-      <c r="F5" s="0" t="s">
+      <c r="G5" s="0" t="s">
         <v>418</v>
       </c>
-      <c r="G5" s="0" t="s">
+      <c r="H5" s="0" t="s">
+        <v>418</v>
+      </c>
+      <c r="I5" s="0" t="s">
+        <v>418</v>
+      </c>
+      <c r="J5" s="0" t="s">
         <v>419</v>
-      </c>
-      <c r="H5" s="0" t="s">
-        <v>419</v>
-      </c>
-      <c r="I5" s="0" t="s">
-        <v>419</v>
-      </c>
-      <c r="J5" s="0" t="s">
-        <v>420</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
+        <v>420</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>399</v>
+      </c>
+      <c r="C6" s="0" t="s">
         <v>421</v>
       </c>
-      <c r="B6" s="0" t="s">
-        <v>422</v>
-      </c>
-      <c r="C6" s="0" t="s">
-        <v>423</v>
-      </c>
       <c r="D6" s="0" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="E6" s="0" t="s">
         <v>100</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="I6" s="0" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="J6" s="0" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
     </row>
   </sheetData>
@@ -3744,7 +3692,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="34.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="9.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="36.57"/>
@@ -3757,88 +3705,88 @@
         <v>0</v>
       </c>
       <c r="B1" s="9" t="s">
+        <v>424</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>425</v>
+      </c>
+      <c r="D1" s="9" t="s">
         <v>426</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="E1" s="9" t="s">
         <v>427</v>
-      </c>
-      <c r="D1" s="9" t="s">
-        <v>428</v>
-      </c>
-      <c r="E1" s="9" t="s">
-        <v>429</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
+        <v>430</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>431</v>
+      </c>
+      <c r="C3" s="0" t="s">
         <v>432</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="D3" s="0" t="s">
         <v>433</v>
-      </c>
-      <c r="C3" s="0" t="s">
-        <v>315</v>
-      </c>
-      <c r="D3" s="0" t="s">
-        <v>434</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
+        <v>434</v>
+      </c>
+      <c r="B4" s="0" t="s">
         <v>435</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="D4" s="0" t="s">
         <v>436</v>
       </c>
-      <c r="D4" s="0" t="s">
-        <v>437</v>
-      </c>
       <c r="E4" s="0" t="s">
-        <v>315</v>
+        <v>432</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
+        <v>437</v>
+      </c>
+      <c r="B5" s="0" t="s">
         <v>438</v>
-      </c>
-      <c r="B5" s="0" t="s">
-        <v>439</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
+        <v>439</v>
+      </c>
+      <c r="B6" s="0" t="s">
         <v>440</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="C6" s="0" t="s">
+        <v>432</v>
+      </c>
+      <c r="D6" s="0" t="s">
         <v>441</v>
-      </c>
-      <c r="C6" s="0" t="s">
-        <v>315</v>
-      </c>
-      <c r="D6" s="0" t="s">
-        <v>442</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
+        <v>442</v>
+      </c>
+      <c r="B7" s="0" t="s">
         <v>443</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="D7" s="0" t="s">
         <v>444</v>
       </c>
-      <c r="D7" s="0" t="s">
-        <v>445</v>
-      </c>
       <c r="E7" s="0" t="s">
-        <v>315</v>
+        <v>432</v>
       </c>
     </row>
   </sheetData>
@@ -3862,7 +3810,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
+      <selection pane="bottomLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3880,65 +3828,68 @@
         <v>112</v>
       </c>
       <c r="C1" s="9" t="s">
+        <v>445</v>
+      </c>
+      <c r="D1" s="9" t="s">
         <v>446</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="E1" s="9" t="s">
         <v>447</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="F1" s="9" t="s">
         <v>448</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="G1" s="9" t="s">
         <v>449</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="H1" s="9" t="s">
         <v>450</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="I1" s="9" t="s">
         <v>451</v>
-      </c>
-      <c r="I1" s="9" t="s">
-        <v>452</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
+        <v>452</v>
+      </c>
+      <c r="B2" s="17" t="s">
         <v>453</v>
       </c>
-      <c r="B2" s="17" t="s">
+      <c r="C2" s="0" t="s">
         <v>454</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="D2" s="0" t="s">
         <v>455</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="F2" s="0" t="s">
         <v>456</v>
       </c>
-      <c r="F2" s="0" t="s">
+      <c r="G2" s="0" t="s">
         <v>457</v>
       </c>
-      <c r="G2" s="0" t="s">
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
         <v>458</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="B3" s="17" t="s">
         <v>459</v>
-      </c>
-      <c r="B3" s="17" t="s">
-        <v>460</v>
       </c>
       <c r="C3" s="0" t="s">
         <v>118</v>
       </c>
       <c r="D3" s="0" t="s">
+        <v>460</v>
+      </c>
+      <c r="E3" s="0" t="s">
         <v>461</v>
       </c>
       <c r="F3" s="0" t="s">
+        <v>456</v>
+      </c>
+      <c r="G3" s="0" t="s">
         <v>457</v>
-      </c>
-      <c r="G3" s="0" t="s">
-        <v>458</v>
       </c>
       <c r="H3" s="0" t="s">
         <v>462</v>
@@ -4213,7 +4164,7 @@
         <v>7</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="I1" s="4" t="s">
         <v>504</v>
@@ -4411,10 +4362,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:I1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4452,7 +4403,7 @@
       <c r="H1" s="4"/>
       <c r="I1" s="4"/>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>518</v>
       </c>
@@ -4472,6 +4423,7 @@
         <v>523</v>
       </c>
     </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -4499,7 +4451,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="31.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="18.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="18.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="17.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="14.69"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="13.7"/>
@@ -4741,13 +4693,13 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
+      <selection pane="bottomLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="19.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="37.42"/>
@@ -4757,7 +4709,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="19"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="12.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="14.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="27.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="27.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="22.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="26.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="27.71"/>
@@ -4769,12 +4721,12 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="27.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="25.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="23" style="0" width="19.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="0" width="15.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="0" width="15.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="0" width="16.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="0" width="9.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="0" width="26.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="0" width="20.98"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="0" width="15.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="0" width="15.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="31" style="0" width="16.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="32" style="0" width="8.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="33" style="0" width="26.42"/>
@@ -5239,7 +5191,6 @@
     <oddHeader/>
     <oddFooter/>
   </headerFooter>
-  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -5259,11 +5210,11 @@
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="10.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="41.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="24.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="10" width="19.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="10" width="19.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="24.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="11" width="24.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="15.15"/>
@@ -5642,14 +5593,14 @@
   <dimension ref="A1:P4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G4" activeCellId="0" sqref="G4"/>
+      <selection pane="topLeft" activeCell="P2" activeCellId="0" sqref="P2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="24.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="24.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="22.86"/>
@@ -5716,7 +5667,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>240</v>
       </c>
@@ -5736,77 +5687,77 @@
         <v>0</v>
       </c>
       <c r="G2" s="0" t="s">
+        <v>244</v>
+      </c>
+      <c r="H2" s="0" t="s">
         <v>245</v>
-      </c>
-      <c r="H2" s="0" t="s">
-        <v>246</v>
       </c>
       <c r="I2" s="0" t="s">
         <v>24</v>
       </c>
       <c r="J2" s="0" t="s">
+        <v>246</v>
+      </c>
+      <c r="O2" s="0" t="s">
         <v>247</v>
       </c>
-      <c r="O2" s="0" t="s">
+      <c r="P2" s="0" t="s">
         <v>248</v>
-      </c>
-      <c r="P2" s="0" t="s">
-        <v>249</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
+        <v>249</v>
+      </c>
+      <c r="B3" s="0" t="s">
         <v>250</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="C3" s="0" t="s">
         <v>251</v>
-      </c>
-      <c r="C3" s="0" t="s">
-        <v>252</v>
       </c>
       <c r="F3" s="0" t="n">
         <v>0</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="H3" s="0" t="s">
+        <v>252</v>
+      </c>
+      <c r="I3" s="0" t="s">
         <v>253</v>
       </c>
-      <c r="I3" s="0" t="s">
+      <c r="J3" s="0" t="s">
         <v>254</v>
       </c>
-      <c r="J3" s="0" t="s">
+      <c r="K3" s="0" t="s">
         <v>255</v>
-      </c>
-      <c r="K3" s="0" t="s">
-        <v>256</v>
       </c>
       <c r="L3" s="0" t="n">
         <v>25</v>
       </c>
       <c r="M3" s="0" t="s">
+        <v>256</v>
+      </c>
+      <c r="N3" s="0" t="s">
         <v>257</v>
-      </c>
-      <c r="N3" s="0" t="s">
-        <v>258</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
+        <v>258</v>
+      </c>
+      <c r="B4" s="0" t="s">
         <v>259</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="C4" s="0" t="s">
         <v>260</v>
       </c>
-      <c r="C4" s="0" t="s">
-        <v>261</v>
-      </c>
       <c r="G4" s="0" t="s">
+        <v>244</v>
+      </c>
+      <c r="H4" s="0" t="s">
         <v>245</v>
-      </c>
-      <c r="H4" s="0" t="s">
-        <v>246</v>
       </c>
       <c r="I4" s="0" t="s">
         <v>42</v>
@@ -5859,7 +5810,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C1" s="9" t="s">
         <v>11</v>
@@ -5868,16 +5819,16 @@
         <v>12</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F1" s="9" t="s">
         <v>15</v>
       </c>
       <c r="G1" s="9" t="s">
+        <v>263</v>
+      </c>
+      <c r="H1" s="9" t="s">
         <v>264</v>
-      </c>
-      <c r="H1" s="9" t="s">
-        <v>265</v>
       </c>
       <c r="I1" s="9" t="s">
         <v>21</v>
@@ -5889,21 +5840,21 @@
         <v>113</v>
       </c>
       <c r="L1" s="16" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
+        <v>266</v>
+      </c>
+      <c r="B2" s="0" t="s">
         <v>267</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="C2" s="0" t="s">
         <v>268</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="D2" s="0" t="s">
         <v>269</v>
-      </c>
-      <c r="D2" s="0" t="s">
-        <v>270</v>
       </c>
       <c r="E2" s="0" t="s">
         <v>76</v>
@@ -5924,24 +5875,24 @@
         <v>8867765</v>
       </c>
       <c r="K2" s="0" t="s">
+        <v>270</v>
+      </c>
+      <c r="L2" s="0" t="s">
         <v>271</v>
-      </c>
-      <c r="L2" s="0" t="s">
-        <v>272</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
+        <v>272</v>
+      </c>
+      <c r="B3" s="0" t="s">
         <v>273</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="C3" s="0" t="s">
         <v>274</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="D3" s="0" t="s">
         <v>275</v>
-      </c>
-      <c r="D3" s="0" t="s">
-        <v>276</v>
       </c>
       <c r="E3" s="0" t="s">
         <v>30</v>
@@ -5962,24 +5913,24 @@
         <v>1084566</v>
       </c>
       <c r="K3" s="0" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="L3" s="0" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
+        <v>276</v>
+      </c>
+      <c r="B4" s="0" t="s">
         <v>277</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>278</v>
       </c>
       <c r="C4" s="0" t="s">
         <v>75</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="E4" s="0" t="s">
         <v>76</v>
@@ -6000,7 +5951,7 @@
         <v>45654656</v>
       </c>
       <c r="K4" s="0" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed VC issue and update excel sheet
Signed-off-by: Ankit Jaiswal <ajaiswal@navatargroup.com>
</commit_message>
<xml_diff>
--- a/SmokeTestCases.xlsx
+++ b/SmokeTestCases.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21929"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F22D8E5-D1A0-4E10-9E1C-2E5B04237880}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="622" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="622" firstSheet="13" activeTab="18"/>
   </bookViews>
   <sheets>
     <sheet name="Institutions" sheetId="22" r:id="rId1"/>
@@ -34,12 +33,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="C6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000001000000}">
+    <comment ref="C6" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -69,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="851" uniqueCount="487">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="851" uniqueCount="485">
   <si>
     <t>Variable_Name</t>
   </si>
@@ -128,9 +127,6 @@
     <t>User_Profile</t>
   </si>
   <si>
-    <t>PE Standard User</t>
-  </si>
-  <si>
     <t>Fund_Type</t>
   </si>
   <si>
@@ -1313,120 +1309,12 @@
     <t>Capital_Returned_NonRecallable</t>
   </si>
   <si>
-    <t>10/14/2019</t>
-  </si>
-  <si>
-    <t>FC - 146</t>
-  </si>
-  <si>
-    <t>FC - 147</t>
-  </si>
-  <si>
-    <t>FC - 148</t>
-  </si>
-  <si>
-    <t>FC - 149</t>
-  </si>
-  <si>
-    <t>FC - 150</t>
-  </si>
-  <si>
-    <t>FC - 151</t>
-  </si>
-  <si>
-    <t>FC - 152</t>
-  </si>
-  <si>
-    <t>FC - 153</t>
-  </si>
-  <si>
     <t>20000000</t>
   </si>
   <si>
     <t>10000000</t>
   </si>
   <si>
-    <t>CMT - 000932</t>
-  </si>
-  <si>
-    <t>CMT - 000933</t>
-  </si>
-  <si>
-    <t>CMT - 000934</t>
-  </si>
-  <si>
-    <t>CMT - 000935</t>
-  </si>
-  <si>
-    <t>CMT - 000936</t>
-  </si>
-  <si>
-    <t>deelroom+16569@gmail.com</t>
-  </si>
-  <si>
-    <t>deelroom+91676@gmail.com</t>
-  </si>
-  <si>
-    <t>deelroom+79864@gmail.com</t>
-  </si>
-  <si>
-    <t>deelroom+41020@gmail.com</t>
-  </si>
-  <si>
-    <t>deelroom+15819@gmail.com</t>
-  </si>
-  <si>
-    <t>3/18/2020</t>
-  </si>
-  <si>
-    <t>3/20/2020</t>
-  </si>
-  <si>
-    <t>CMT - 000930</t>
-  </si>
-  <si>
-    <t>CMT - 000931</t>
-  </si>
-  <si>
-    <t>3/22/2020</t>
-  </si>
-  <si>
-    <t>3/23/2020</t>
-  </si>
-  <si>
-    <t>3.75E8</t>
-  </si>
-  <si>
-    <t>3/26/2020</t>
-  </si>
-  <si>
-    <t>3/29/2020</t>
-  </si>
-  <si>
-    <t>2.8E7</t>
-  </si>
-  <si>
-    <t>4/3/2020</t>
-  </si>
-  <si>
-    <t>TestCompany1 - Mar 2020</t>
-  </si>
-  <si>
-    <t>TestCompany2 - Mar 2020</t>
-  </si>
-  <si>
-    <t>TestCompany3 - Mar 2020</t>
-  </si>
-  <si>
-    <t>deelroom+74427@gmail.com</t>
-  </si>
-  <si>
-    <t>deelroom+49521@gmail.com</t>
-  </si>
-  <si>
-    <t>3/19/2020</t>
-  </si>
-  <si>
     <t>400000</t>
   </si>
   <si>
@@ -1439,9 +1327,6 @@
     <t>500,000.000</t>
   </si>
   <si>
-    <t>DD-0215</t>
-  </si>
-  <si>
     <t>CC-0619</t>
   </si>
   <si>
@@ -1454,9 +1339,6 @@
     <t>CC-0622</t>
   </si>
   <si>
-    <t>CC-0623</t>
-  </si>
-  <si>
     <t>25000000</t>
   </si>
   <si>
@@ -1496,9 +1378,6 @@
     <t>2399999.999</t>
   </si>
   <si>
-    <t>FD-0228</t>
-  </si>
-  <si>
     <t>ID-0625</t>
   </si>
   <si>
@@ -1508,37 +1387,151 @@
     <t>ID-0627</t>
   </si>
   <si>
-    <t>ID-0628</t>
-  </si>
-  <si>
-    <t>ID-0629</t>
-  </si>
-  <si>
-    <t>FD-0248</t>
+    <t>VC Standard Profile User</t>
+  </si>
+  <si>
+    <t>CustomReportFolder33167</t>
+  </si>
+  <si>
+    <t>CustomReport27301</t>
+  </si>
+  <si>
+    <t>PETestEmailFolder18888</t>
+  </si>
+  <si>
+    <t>PETestCustomEmailTemplate36540</t>
+  </si>
+  <si>
+    <t>deelroom+88755@gmail.com</t>
+  </si>
+  <si>
+    <t>deelroom+58133@gmail.com</t>
+  </si>
+  <si>
+    <t>deelroom+96564@gmail.com</t>
+  </si>
+  <si>
+    <t>deelroom+86783@gmail.com</t>
+  </si>
+  <si>
+    <t>deelroom+41003@gmail.com</t>
+  </si>
+  <si>
+    <t>7/16/2020</t>
+  </si>
+  <si>
+    <t>FC - 136</t>
+  </si>
+  <si>
+    <t>FC - 137</t>
+  </si>
+  <si>
+    <t>FC - 138</t>
+  </si>
+  <si>
+    <t>FC - 139</t>
+  </si>
+  <si>
+    <t>FC - 140</t>
+  </si>
+  <si>
+    <t>FC - 141</t>
+  </si>
+  <si>
+    <t>FC - 142</t>
+  </si>
+  <si>
+    <t>FC - 143</t>
+  </si>
+  <si>
+    <t>7/17/2020</t>
+  </si>
+  <si>
+    <t>7/18/2020</t>
+  </si>
+  <si>
+    <t>CMT - 000922</t>
+  </si>
+  <si>
+    <t>CMT - 000923</t>
+  </si>
+  <si>
+    <t>7/20/2020</t>
+  </si>
+  <si>
+    <t>7/21/2020</t>
+  </si>
+  <si>
+    <t>CMT - 000924</t>
+  </si>
+  <si>
+    <t>CMT - 000925</t>
+  </si>
+  <si>
+    <t>4.5E8</t>
+  </si>
+  <si>
+    <t>7/24/2020</t>
+  </si>
+  <si>
+    <t>CMT - 000926</t>
+  </si>
+  <si>
+    <t>7/27/2020</t>
+  </si>
+  <si>
+    <t>CMT - 000927</t>
+  </si>
+  <si>
+    <t>4.2E7</t>
+  </si>
+  <si>
+    <t>8/1/2020</t>
+  </si>
+  <si>
+    <t>CMT - 000928</t>
+  </si>
+  <si>
+    <t>TestCompany1 - Jul 2020</t>
+  </si>
+  <si>
+    <t>TestCompany2 - Jul 2020</t>
+  </si>
+  <si>
+    <t>TestCompany3 - Jul 2020</t>
+  </si>
+  <si>
+    <t>deelroom+74310@gmail.com</t>
+  </si>
+  <si>
+    <t>deelroom+91109@gmail.com</t>
+  </si>
+  <si>
+    <t>DD-0214</t>
+  </si>
+  <si>
+    <t>CC-0618</t>
+  </si>
+  <si>
+    <t>FD-0226</t>
+  </si>
+  <si>
+    <t>ID-0623</t>
+  </si>
+  <si>
+    <t>ID-0624</t>
   </si>
   <si>
     <t>User</t>
-  </si>
-  <si>
-    <t>PETestEmailFolder</t>
-  </si>
-  <si>
-    <t>PETestCustomEmailTemplate</t>
-  </si>
-  <si>
-    <t>CustomReportFolder</t>
-  </si>
-  <si>
-    <t>CustomReport</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
-    <numFmt numFmtId="165" formatCode="mm/dd/yy;@"/>
+    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
+    <numFmt numFmtId="164" formatCode="mm/dd/yy;@"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -1630,10 +1623,10 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1648,7 +1641,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
@@ -1953,10 +1946,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B20" sqref="B20"/>
     </sheetView>
@@ -1995,104 +1988,104 @@
         <v>1</v>
       </c>
       <c r="C1" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>167</v>
+      </c>
+      <c r="F1" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="G1" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="I1" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="E1" s="7" t="s">
-        <v>168</v>
-      </c>
-      <c r="F1" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="G1" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="H1" s="7" t="s">
+      <c r="J1" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="K1" s="7" t="s">
+        <v>357</v>
+      </c>
+      <c r="L1" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="M1" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="N1" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="O1" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="P1" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="Q1" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="R1" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="S1" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="T1" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="U1" s="7" t="s">
+        <v>366</v>
+      </c>
+      <c r="V1" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="W1" s="7" t="s">
         <v>32</v>
-      </c>
-      <c r="I1" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="J1" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="K1" s="7" t="s">
-        <v>358</v>
-      </c>
-      <c r="L1" s="7" t="s">
-        <v>135</v>
-      </c>
-      <c r="M1" s="7" t="s">
-        <v>134</v>
-      </c>
-      <c r="N1" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="O1" s="7" t="s">
-        <v>136</v>
-      </c>
-      <c r="P1" s="7" t="s">
-        <v>137</v>
-      </c>
-      <c r="Q1" s="7" t="s">
-        <v>138</v>
-      </c>
-      <c r="R1" s="7" t="s">
-        <v>139</v>
-      </c>
-      <c r="S1" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="T1" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="U1" s="7" t="s">
-        <v>367</v>
-      </c>
-      <c r="V1" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="W1" s="7" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" t="s">
         <v>34</v>
-      </c>
-      <c r="C2" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3" t="s">
+        <v>34</v>
+      </c>
+      <c r="L3" t="s">
         <v>41</v>
       </c>
-      <c r="C3" t="s">
-        <v>35</v>
-      </c>
-      <c r="L3" t="s">
+      <c r="M3" t="s">
         <v>42</v>
       </c>
-      <c r="M3" t="s">
+      <c r="N3" t="s">
         <v>43</v>
-      </c>
-      <c r="N3" t="s">
-        <v>44</v>
       </c>
       <c r="O3">
         <v>210310</v>
       </c>
       <c r="P3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="V3">
         <v>3636366336</v>
@@ -2103,39 +2096,39 @@
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C5" t="s">
+        <v>34</v>
+      </c>
+      <c r="L5" t="s">
         <v>48</v>
       </c>
-      <c r="C5" t="s">
-        <v>35</v>
-      </c>
-      <c r="L5" t="s">
+      <c r="M5" t="s">
         <v>49</v>
       </c>
-      <c r="M5" t="s">
+      <c r="N5" t="s">
         <v>50</v>
-      </c>
-      <c r="N5" t="s">
-        <v>51</v>
       </c>
       <c r="O5">
         <v>900268</v>
       </c>
       <c r="P5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="V5">
         <v>66228811</v>
@@ -2146,180 +2139,180 @@
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7" t="s">
         <v>36</v>
-      </c>
-      <c r="C7" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B10" t="s">
+        <v>37</v>
+      </c>
+      <c r="C10" t="s">
         <v>38</v>
-      </c>
-      <c r="C10" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B12" t="s">
+        <v>315</v>
+      </c>
+      <c r="C12" t="s">
+        <v>36</v>
+      </c>
+      <c r="H12" t="s">
         <v>316</v>
       </c>
-      <c r="C12" t="s">
-        <v>37</v>
-      </c>
-      <c r="H12" t="s">
+      <c r="I12" t="s">
         <v>317</v>
       </c>
-      <c r="I12" t="s">
+      <c r="J12" t="s">
         <v>318</v>
       </c>
-      <c r="J12" t="s">
+      <c r="K12" t="s">
         <v>319</v>
       </c>
-      <c r="K12" t="s">
+      <c r="L12" t="s">
         <v>320</v>
       </c>
-      <c r="L12" t="s">
-        <v>321</v>
-      </c>
       <c r="M12" t="s">
+        <v>42</v>
+      </c>
+      <c r="N12" t="s">
         <v>43</v>
-      </c>
-      <c r="N12" t="s">
-        <v>44</v>
       </c>
       <c r="O12">
         <v>281001</v>
       </c>
       <c r="P12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="Q12" t="s">
+        <v>321</v>
+      </c>
+      <c r="R12" t="s">
         <v>322</v>
       </c>
-      <c r="R12" t="s">
+      <c r="S12" t="s">
         <v>323</v>
-      </c>
-      <c r="S12" t="s">
-        <v>324</v>
       </c>
       <c r="T12">
         <v>200300</v>
       </c>
       <c r="U12" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="V12">
         <v>2121212121</v>
       </c>
       <c r="W12" s="15" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B13" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H13" t="s">
+        <v>325</v>
+      </c>
+      <c r="I13" t="s">
+        <v>317</v>
+      </c>
+      <c r="J13" t="s">
+        <v>318</v>
+      </c>
+      <c r="K13" t="s">
+        <v>319</v>
+      </c>
+      <c r="L13" t="s">
         <v>326</v>
       </c>
-      <c r="I13" t="s">
-        <v>318</v>
-      </c>
-      <c r="J13" t="s">
-        <v>319</v>
-      </c>
-      <c r="K13" t="s">
-        <v>320</v>
-      </c>
-      <c r="L13" t="s">
+      <c r="M13" t="s">
         <v>327</v>
       </c>
-      <c r="M13" t="s">
-        <v>328</v>
-      </c>
       <c r="N13" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="O13">
         <v>201301</v>
       </c>
       <c r="P13" t="s">
+        <v>328</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>371</v>
+      </c>
+      <c r="R13" t="s">
         <v>329</v>
       </c>
-      <c r="Q13" t="s">
-        <v>372</v>
-      </c>
-      <c r="R13" t="s">
-        <v>330</v>
-      </c>
       <c r="S13" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="T13">
         <v>10016</v>
       </c>
       <c r="U13" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="V13">
         <v>98765429</v>
@@ -2327,55 +2320,55 @@
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B14" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C14" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H14" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="I14" t="s">
+        <v>317</v>
+      </c>
+      <c r="J14" t="s">
         <v>318</v>
       </c>
-      <c r="J14" t="s">
+      <c r="K14" t="s">
         <v>319</v>
       </c>
-      <c r="K14" t="s">
-        <v>320</v>
-      </c>
       <c r="L14" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="M14" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="N14" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="O14">
         <v>500700</v>
       </c>
       <c r="P14" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="Q14" t="s">
+        <v>332</v>
+      </c>
+      <c r="R14" t="s">
         <v>333</v>
       </c>
-      <c r="R14" t="s">
-        <v>334</v>
-      </c>
       <c r="S14" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="T14">
         <v>2834</v>
       </c>
       <c r="U14" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="V14">
         <v>1629539588</v>
@@ -2383,58 +2376,58 @@
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B15" t="s">
+        <v>335</v>
+      </c>
+      <c r="C15" t="s">
+        <v>36</v>
+      </c>
+      <c r="E15" s="2" t="s">
         <v>336</v>
       </c>
-      <c r="C15" t="s">
-        <v>37</v>
-      </c>
-      <c r="E15" s="2" t="s">
+      <c r="H15" t="s">
         <v>337</v>
       </c>
-      <c r="H15" t="s">
+      <c r="I15" t="s">
+        <v>317</v>
+      </c>
+      <c r="J15" t="s">
         <v>338</v>
       </c>
-      <c r="I15" t="s">
-        <v>318</v>
-      </c>
-      <c r="J15" t="s">
+      <c r="K15" t="s">
         <v>339</v>
       </c>
-      <c r="K15" t="s">
+      <c r="L15" t="s">
         <v>340</v>
       </c>
-      <c r="L15" t="s">
+      <c r="M15" t="s">
+        <v>388</v>
+      </c>
+      <c r="N15" t="s">
         <v>341</v>
-      </c>
-      <c r="M15" t="s">
-        <v>389</v>
-      </c>
-      <c r="N15" t="s">
-        <v>342</v>
       </c>
       <c r="O15">
         <v>560003</v>
       </c>
       <c r="P15" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="Q15" t="s">
+        <v>340</v>
+      </c>
+      <c r="R15" t="s">
+        <v>388</v>
+      </c>
+      <c r="S15" t="s">
         <v>341</v>
-      </c>
-      <c r="R15" t="s">
-        <v>389</v>
-      </c>
-      <c r="S15" t="s">
-        <v>342</v>
       </c>
       <c r="T15">
         <v>560003</v>
       </c>
       <c r="U15" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="V15">
         <v>9999999999</v>
@@ -2442,7 +2435,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E15" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="E15" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
@@ -2450,7 +2443,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2477,54 +2470,54 @@
         <v>5</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>261</v>
+      </c>
+      <c r="B2" t="s">
         <v>262</v>
       </c>
-      <c r="B2" t="s">
-        <v>263</v>
-      </c>
       <c r="C2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>263</v>
+      </c>
+      <c r="B3" t="s">
         <v>264</v>
       </c>
-      <c r="B3" t="s">
-        <v>265</v>
-      </c>
       <c r="C3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D3" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>265</v>
+      </c>
+      <c r="B4" t="s">
         <v>266</v>
       </c>
-      <c r="B4" t="s">
-        <v>267</v>
-      </c>
       <c r="C4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>267</v>
+      </c>
+      <c r="B5" t="s">
         <v>268</v>
       </c>
-      <c r="B5" t="s">
-        <v>269</v>
-      </c>
       <c r="C5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -2533,7 +2526,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T10"/>
   <sheetViews>
     <sheetView topLeftCell="M1" workbookViewId="0">
@@ -2570,138 +2563,138 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D1" s="3" t="s">
+        <v>269</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>270</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
+        <v>314</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>313</v>
+      </c>
+      <c r="H1" s="3" t="s">
         <v>271</v>
       </c>
-      <c r="F1" s="3" t="s">
-        <v>315</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>314</v>
-      </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="J1" s="3" t="s">
         <v>272</v>
       </c>
-      <c r="I1" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="19" t="s">
         <v>273</v>
       </c>
-      <c r="K1" s="19" t="s">
+      <c r="L1" s="19" t="s">
         <v>274</v>
       </c>
-      <c r="L1" s="19" t="s">
+      <c r="M1" s="19" t="s">
         <v>275</v>
       </c>
-      <c r="M1" s="19" t="s">
+      <c r="N1" s="19" t="s">
         <v>276</v>
       </c>
-      <c r="N1" s="19" t="s">
+      <c r="O1" s="3" t="s">
         <v>277</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="P1" s="3" t="s">
         <v>278</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="Q1" s="16" t="s">
+        <v>400</v>
+      </c>
+      <c r="R1" s="26" t="s">
+        <v>411</v>
+      </c>
+      <c r="S1" s="16" t="s">
+        <v>412</v>
+      </c>
+      <c r="T1" s="3" t="s">
         <v>279</v>
-      </c>
-      <c r="Q1" s="16" t="s">
-        <v>401</v>
-      </c>
-      <c r="R1" s="26" t="s">
-        <v>412</v>
-      </c>
-      <c r="S1" s="16" t="s">
-        <v>413</v>
-      </c>
-      <c r="T1" s="3" t="s">
-        <v>280</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B2" t="s">
-        <v>437</v>
+        <v>460</v>
       </c>
       <c r="C2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D2" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="E2">
         <v>20000000</v>
       </c>
       <c r="F2" t="s">
+        <v>281</v>
+      </c>
+      <c r="G2" t="s">
         <v>282</v>
       </c>
-      <c r="G2" t="s">
-        <v>283</v>
-      </c>
       <c r="H2" t="s">
-        <v>435</v>
+        <v>458</v>
       </c>
       <c r="P2" s="18"/>
       <c r="T2" s="28" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B3" t="s">
-        <v>438</v>
+        <v>461</v>
       </c>
       <c r="C3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D3" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="E3">
         <v>10000000</v>
       </c>
       <c r="F3" t="s">
+        <v>281</v>
+      </c>
+      <c r="G3" t="s">
         <v>282</v>
       </c>
-      <c r="G3" t="s">
-        <v>283</v>
-      </c>
       <c r="H3" t="s">
-        <v>436</v>
+        <v>459</v>
       </c>
       <c r="T3" s="28"/>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B4" t="s">
-        <v>425</v>
+        <v>464</v>
       </c>
       <c r="C4" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D4" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="E4">
         <v>15000000</v>
       </c>
       <c r="H4" t="s">
-        <v>439</v>
+        <v>462</v>
       </c>
       <c r="J4">
         <v>7.5</v>
@@ -2710,22 +2703,22 @@
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B5" t="s">
-        <v>426</v>
+        <v>465</v>
       </c>
       <c r="C5" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D5" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="E5">
         <v>25000000</v>
       </c>
       <c r="H5" t="s">
-        <v>440</v>
+        <v>463</v>
       </c>
       <c r="J5">
         <v>7.5</v>
@@ -2734,100 +2727,100 @@
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B6" t="s">
-        <v>427</v>
+        <v>468</v>
       </c>
       <c r="C6" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D6" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="E6">
         <v>5000000</v>
       </c>
       <c r="H6" t="s">
-        <v>442</v>
+        <v>467</v>
       </c>
       <c r="T6" s="28"/>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B7" t="s">
-        <v>428</v>
+        <v>470</v>
       </c>
       <c r="C7" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D7" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="E7">
         <v>2000000</v>
       </c>
       <c r="H7" t="s">
-        <v>443</v>
+        <v>469</v>
       </c>
       <c r="I7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="T7" s="28"/>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="B8" t="s">
-        <v>429</v>
+        <v>473</v>
       </c>
       <c r="C8" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D8" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="E8">
         <v>12000000</v>
       </c>
       <c r="H8" t="s">
-        <v>445</v>
+        <v>472</v>
       </c>
       <c r="I8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="T8" s="28"/>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B9" t="s">
-        <v>437</v>
+        <v>460</v>
       </c>
       <c r="C9" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D9" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="E9">
         <v>20000000</v>
       </c>
       <c r="F9" t="s">
+        <v>281</v>
+      </c>
+      <c r="G9" t="s">
         <v>282</v>
       </c>
-      <c r="G9" t="s">
-        <v>283</v>
-      </c>
       <c r="H9" t="s">
-        <v>435</v>
+        <v>458</v>
       </c>
       <c r="K9" s="14" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="L9" s="14">
         <v>2000000</v>
@@ -2839,48 +2832,48 @@
         <v>0</v>
       </c>
       <c r="O9" s="14" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="P9" s="14">
         <v>0</v>
       </c>
       <c r="Q9" s="15" t="s">
+        <v>409</v>
+      </c>
+      <c r="R9" s="15" t="s">
         <v>410</v>
-      </c>
-      <c r="R9" s="15" t="s">
-        <v>411</v>
       </c>
       <c r="S9">
         <v>0</v>
       </c>
       <c r="T9" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B10" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C10" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D10" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="E10">
         <v>20000000</v>
       </c>
       <c r="F10" t="s">
+        <v>281</v>
+      </c>
+      <c r="G10" t="s">
         <v>282</v>
       </c>
-      <c r="G10" t="s">
-        <v>283</v>
-      </c>
       <c r="H10" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="K10" s="15">
         <v>2000000</v>
@@ -2895,7 +2888,7 @@
         <v>0</v>
       </c>
       <c r="O10" s="14" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="P10" s="14">
         <v>0</v>
@@ -2910,7 +2903,7 @@
         <v>0</v>
       </c>
       <c r="T10" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
   </sheetData>
@@ -2923,7 +2916,7 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2949,245 +2942,245 @@
         <v>0</v>
       </c>
       <c r="B1" s="19" t="s">
+        <v>294</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>292</v>
+      </c>
+      <c r="D1" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" s="19" t="s">
         <v>295</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>293</v>
-      </c>
-      <c r="D1" s="19" t="s">
-        <v>21</v>
-      </c>
-      <c r="E1" s="19" t="s">
+      <c r="F1" s="19" t="s">
         <v>296</v>
       </c>
-      <c r="F1" s="19" t="s">
+      <c r="G1" s="19" t="s">
         <v>297</v>
       </c>
-      <c r="G1" s="19" t="s">
+      <c r="H1" s="19" t="s">
         <v>298</v>
       </c>
-      <c r="H1" s="19" t="s">
+      <c r="I1" s="19" t="s">
         <v>299</v>
       </c>
-      <c r="I1" s="19" t="s">
+      <c r="J1" s="19" t="s">
         <v>300</v>
       </c>
-      <c r="J1" s="19" t="s">
+      <c r="K1" s="19" t="s">
         <v>301</v>
       </c>
-      <c r="K1" s="19" t="s">
+      <c r="L1" s="19" t="s">
         <v>302</v>
       </c>
-      <c r="L1" s="19" t="s">
+      <c r="M1" s="19" t="s">
         <v>303</v>
-      </c>
-      <c r="M1" s="19" t="s">
-        <v>304</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B2" t="s">
-        <v>457</v>
+        <v>480</v>
       </c>
       <c r="C2" t="s">
-        <v>456</v>
+        <v>479</v>
       </c>
       <c r="D2" t="s">
-        <v>426</v>
+        <v>465</v>
       </c>
       <c r="E2" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="F2" t="s">
+        <v>383</v>
+      </c>
+      <c r="G2" t="s">
+        <v>383</v>
+      </c>
+      <c r="H2" t="s">
         <v>384</v>
       </c>
-      <c r="G2" t="s">
-        <v>384</v>
-      </c>
-      <c r="H2" t="s">
-        <v>385</v>
-      </c>
       <c r="I2" t="s">
-        <v>451</v>
+        <v>458</v>
       </c>
       <c r="J2" t="s">
-        <v>436</v>
+        <v>459</v>
       </c>
       <c r="K2" s="15" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="L2" s="21" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="M2" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B3" t="s">
+        <v>419</v>
+      </c>
+      <c r="C3" t="s">
+        <v>479</v>
+      </c>
+      <c r="D3" t="s">
+        <v>468</v>
+      </c>
+      <c r="E3" t="s">
+        <v>415</v>
+      </c>
+      <c r="F3" t="s">
+        <v>416</v>
+      </c>
+      <c r="G3" t="s">
+        <v>416</v>
+      </c>
+      <c r="H3" t="s">
+        <v>417</v>
+      </c>
+      <c r="I3" t="s">
         <v>458</v>
       </c>
-      <c r="C3" t="s">
-        <v>456</v>
-      </c>
-      <c r="D3" t="s">
-        <v>427</v>
-      </c>
-      <c r="E3" t="s">
-        <v>452</v>
-      </c>
-      <c r="F3" t="s">
-        <v>453</v>
-      </c>
-      <c r="G3" t="s">
-        <v>453</v>
-      </c>
-      <c r="H3" t="s">
-        <v>454</v>
-      </c>
-      <c r="I3" t="s">
-        <v>451</v>
-      </c>
       <c r="J3" t="s">
-        <v>436</v>
+        <v>459</v>
       </c>
       <c r="K3" s="15" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="L3" s="15" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="M3" t="s">
-        <v>455</v>
+        <v>418</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B4" t="s">
+        <v>420</v>
+      </c>
+      <c r="C4" t="s">
+        <v>479</v>
+      </c>
+      <c r="D4" t="s">
+        <v>460</v>
+      </c>
+      <c r="E4" t="s">
+        <v>374</v>
+      </c>
+      <c r="F4" t="s">
+        <v>375</v>
+      </c>
+      <c r="G4" t="s">
+        <v>375</v>
+      </c>
+      <c r="H4" t="s">
+        <v>376</v>
+      </c>
+      <c r="I4" t="s">
+        <v>458</v>
+      </c>
+      <c r="J4" t="s">
         <v>459</v>
       </c>
-      <c r="C4" t="s">
-        <v>456</v>
-      </c>
-      <c r="D4" t="s">
-        <v>437</v>
-      </c>
-      <c r="E4" t="s">
-        <v>375</v>
-      </c>
-      <c r="F4" t="s">
+      <c r="K4" t="s">
         <v>376</v>
       </c>
-      <c r="G4" t="s">
-        <v>376</v>
-      </c>
-      <c r="H4" t="s">
-        <v>377</v>
-      </c>
-      <c r="I4" t="s">
-        <v>451</v>
-      </c>
-      <c r="J4" t="s">
-        <v>436</v>
-      </c>
-      <c r="K4" t="s">
-        <v>377</v>
-      </c>
       <c r="L4" t="s">
-        <v>451</v>
+        <v>458</v>
       </c>
       <c r="M4" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B5" t="s">
-        <v>460</v>
+        <v>421</v>
       </c>
       <c r="C5" t="s">
-        <v>456</v>
+        <v>479</v>
       </c>
       <c r="D5" t="s">
-        <v>425</v>
+        <v>464</v>
       </c>
       <c r="E5" t="s">
+        <v>380</v>
+      </c>
+      <c r="F5" t="s">
         <v>381</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
+        <v>381</v>
+      </c>
+      <c r="H5" t="s">
         <v>382</v>
       </c>
-      <c r="G5" t="s">
-        <v>382</v>
-      </c>
-      <c r="H5" t="s">
-        <v>383</v>
-      </c>
       <c r="I5" t="s">
-        <v>451</v>
+        <v>458</v>
       </c>
       <c r="J5" t="s">
-        <v>436</v>
+        <v>459</v>
       </c>
       <c r="K5" s="14" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="L5" s="14" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="M5" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="15" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B6" t="s">
+        <v>422</v>
+      </c>
+      <c r="C6" t="s">
+        <v>479</v>
+      </c>
+      <c r="D6" t="s">
         <v>461</v>
       </c>
-      <c r="C6" t="s">
-        <v>456</v>
-      </c>
-      <c r="D6" t="s">
-        <v>438</v>
-      </c>
       <c r="E6" t="s">
+        <v>377</v>
+      </c>
+      <c r="F6" t="s">
         <v>378</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
+        <v>378</v>
+      </c>
+      <c r="H6" t="s">
         <v>379</v>
       </c>
-      <c r="G6" t="s">
-        <v>379</v>
-      </c>
-      <c r="H6" t="s">
-        <v>380</v>
-      </c>
       <c r="I6" t="s">
-        <v>451</v>
+        <v>458</v>
       </c>
       <c r="J6" t="s">
-        <v>436</v>
+        <v>459</v>
       </c>
       <c r="K6" s="15" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="L6" s="15" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="M6" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
   </sheetData>
@@ -3196,7 +3189,7 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3222,66 +3215,66 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D1" s="3" t="s">
+        <v>298</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>299</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>300</v>
       </c>
-      <c r="F1" s="3" t="s">
-        <v>301</v>
-      </c>
       <c r="G1" s="3" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="I1" s="3" t="s">
+        <v>295</v>
+      </c>
+      <c r="J1" s="3" t="s">
         <v>296</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>297</v>
       </c>
-      <c r="K1" s="3" t="s">
-        <v>298</v>
-      </c>
       <c r="L1" s="3" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="M1" s="3" t="s">
+        <v>390</v>
+      </c>
+      <c r="N1" s="3" t="s">
         <v>391</v>
       </c>
-      <c r="N1" s="3" t="s">
-        <v>392</v>
-      </c>
       <c r="O1" s="3" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B2" t="s">
-        <v>456</v>
+        <v>479</v>
       </c>
       <c r="C2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="E2" t="s">
-        <v>451</v>
+        <v>458</v>
       </c>
       <c r="F2" t="s">
-        <v>436</v>
+        <v>459</v>
       </c>
       <c r="G2" s="14">
         <v>5500000</v>
@@ -3290,16 +3283,16 @@
         <v>2000000</v>
       </c>
       <c r="I2" s="14" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="J2" s="14" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="K2" s="14">
         <v>750000</v>
       </c>
       <c r="L2" s="15" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="M2" s="15">
         <v>0</v>
@@ -3317,7 +3310,7 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3340,48 +3333,48 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D1" s="3" t="s">
+        <v>396</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>397</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
+        <v>300</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>398</v>
       </c>
-      <c r="F1" s="3" t="s">
-        <v>301</v>
-      </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="I1" s="3" t="s">
         <v>399</v>
       </c>
-      <c r="H1" s="3" t="s">
-        <v>297</v>
-      </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>400</v>
       </c>
-      <c r="J1" s="3" t="s">
-        <v>401</v>
-      </c>
       <c r="K1" s="3" t="s">
+        <v>390</v>
+      </c>
+      <c r="L1" s="3" t="s">
         <v>391</v>
       </c>
-      <c r="L1" s="3" t="s">
-        <v>392</v>
-      </c>
       <c r="M1" s="3" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="B2" t="s">
-        <v>475</v>
+        <v>481</v>
       </c>
       <c r="D2">
         <v>15000000</v>
@@ -3402,7 +3395,7 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3426,200 +3419,200 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>401</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>402</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>403</v>
-      </c>
       <c r="D1" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E1" s="25" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="F1" s="3" t="s">
+        <v>396</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>397</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>398</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>399</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>400</v>
       </c>
-      <c r="J1" s="3" t="s">
-        <v>401</v>
-      </c>
       <c r="M1" s="3" t="s">
+        <v>390</v>
+      </c>
+      <c r="N1" s="3" t="s">
         <v>391</v>
       </c>
-      <c r="N1" s="3" t="s">
-        <v>392</v>
-      </c>
       <c r="O1" s="3" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="B2" t="s">
-        <v>475</v>
+        <v>481</v>
       </c>
       <c r="C2" t="s">
-        <v>476</v>
+        <v>482</v>
       </c>
       <c r="D2" t="s">
+        <v>465</v>
+      </c>
+      <c r="E2" t="s">
+        <v>423</v>
+      </c>
+      <c r="F2" t="s">
+        <v>424</v>
+      </c>
+      <c r="G2" t="s">
+        <v>425</v>
+      </c>
+      <c r="H2" t="s">
+        <v>425</v>
+      </c>
+      <c r="I2" t="s">
+        <v>425</v>
+      </c>
+      <c r="J2" t="s">
         <v>426</v>
-      </c>
-      <c r="E2" t="s">
-        <v>462</v>
-      </c>
-      <c r="F2" t="s">
-        <v>463</v>
-      </c>
-      <c r="G2" t="s">
-        <v>464</v>
-      </c>
-      <c r="H2" t="s">
-        <v>464</v>
-      </c>
-      <c r="I2" t="s">
-        <v>464</v>
-      </c>
-      <c r="J2" t="s">
-        <v>465</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="B3" t="s">
-        <v>475</v>
+        <v>481</v>
       </c>
       <c r="C3" t="s">
-        <v>477</v>
+        <v>483</v>
       </c>
       <c r="D3" t="s">
+        <v>468</v>
+      </c>
+      <c r="E3" t="s">
+        <v>424</v>
+      </c>
+      <c r="F3" t="s">
+        <v>379</v>
+      </c>
+      <c r="G3" t="s">
         <v>427</v>
       </c>
-      <c r="E3" t="s">
-        <v>463</v>
-      </c>
-      <c r="F3" t="s">
-        <v>380</v>
-      </c>
-      <c r="G3" t="s">
-        <v>466</v>
-      </c>
       <c r="H3" t="s">
-        <v>466</v>
+        <v>427</v>
       </c>
       <c r="I3" t="s">
-        <v>466</v>
+        <v>427</v>
       </c>
       <c r="J3" t="s">
-        <v>467</v>
+        <v>428</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="B4" t="s">
-        <v>475</v>
+        <v>481</v>
       </c>
       <c r="C4" t="s">
-        <v>478</v>
+        <v>436</v>
       </c>
       <c r="D4" t="s">
-        <v>437</v>
+        <v>460</v>
       </c>
       <c r="E4" t="s">
-        <v>423</v>
+        <v>413</v>
       </c>
       <c r="F4" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="G4" t="s">
-        <v>468</v>
+        <v>429</v>
       </c>
       <c r="H4" t="s">
-        <v>468</v>
+        <v>429</v>
       </c>
       <c r="I4" t="s">
-        <v>468</v>
+        <v>429</v>
       </c>
       <c r="J4" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B5" t="s">
-        <v>475</v>
+        <v>481</v>
       </c>
       <c r="C5" t="s">
-        <v>479</v>
+        <v>437</v>
       </c>
       <c r="D5" t="s">
-        <v>425</v>
+        <v>464</v>
       </c>
       <c r="E5" t="s">
-        <v>469</v>
+        <v>430</v>
       </c>
       <c r="F5" t="s">
-        <v>470</v>
+        <v>431</v>
       </c>
       <c r="G5" t="s">
-        <v>471</v>
+        <v>432</v>
       </c>
       <c r="H5" t="s">
-        <v>471</v>
+        <v>432</v>
       </c>
       <c r="I5" t="s">
-        <v>471</v>
+        <v>432</v>
       </c>
       <c r="J5" t="s">
-        <v>472</v>
+        <v>433</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="B6" t="s">
         <v>481</v>
       </c>
       <c r="C6" t="s">
-        <v>480</v>
+        <v>438</v>
       </c>
       <c r="D6" t="s">
-        <v>438</v>
+        <v>461</v>
       </c>
       <c r="E6" t="s">
-        <v>424</v>
+        <v>414</v>
       </c>
       <c r="F6" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="G6" t="s">
-        <v>473</v>
+        <v>434</v>
       </c>
       <c r="H6" t="s">
-        <v>473</v>
+        <v>434</v>
       </c>
       <c r="I6" t="s">
-        <v>473</v>
+        <v>434</v>
       </c>
       <c r="J6" t="s">
-        <v>474</v>
+        <v>435</v>
       </c>
     </row>
   </sheetData>
@@ -3628,7 +3621,7 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3649,88 +3642,88 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>202</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>203</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>204</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>204</v>
+      </c>
+      <c r="B2" t="s">
         <v>205</v>
-      </c>
-      <c r="B2" t="s">
-        <v>206</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>206</v>
+      </c>
+      <c r="B3" t="s">
         <v>207</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
+        <v>459</v>
+      </c>
+      <c r="D3" t="s">
         <v>208</v>
-      </c>
-      <c r="C3" t="s">
-        <v>436</v>
-      </c>
-      <c r="D3" t="s">
-        <v>209</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>209</v>
+      </c>
+      <c r="B4" t="s">
         <v>210</v>
       </c>
-      <c r="B4" t="s">
+      <c r="D4" t="s">
         <v>211</v>
       </c>
-      <c r="D4" t="s">
-        <v>212</v>
-      </c>
       <c r="E4" t="s">
-        <v>436</v>
+        <v>459</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>233</v>
+      </c>
+      <c r="B5" t="s">
         <v>234</v>
-      </c>
-      <c r="B5" t="s">
-        <v>235</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>235</v>
+      </c>
+      <c r="B6" t="s">
         <v>236</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
+        <v>459</v>
+      </c>
+      <c r="D6" t="s">
         <v>237</v>
-      </c>
-      <c r="C6" t="s">
-        <v>436</v>
-      </c>
-      <c r="D6" t="s">
-        <v>238</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>238</v>
+      </c>
+      <c r="B7" t="s">
         <v>239</v>
       </c>
-      <c r="B7" t="s">
+      <c r="D7" t="s">
         <v>240</v>
       </c>
-      <c r="D7" t="s">
-        <v>241</v>
-      </c>
       <c r="E7" t="s">
-        <v>436</v>
+        <v>459</v>
       </c>
     </row>
   </sheetData>
@@ -3739,19 +3732,20 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C18" sqref="C18"/>
+      <selection pane="bottomLeft" activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="19" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="4" width="19" collapsed="1"/>
     <col min="5" max="5" width="37.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="16384" width="19" collapsed="1"/>
+    <col min="6" max="6" width="24.42578125" customWidth="1" collapsed="1"/>
+    <col min="7" max="16384" width="19" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -3777,10 +3771,10 @@
         <v>17</v>
       </c>
       <c r="H1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="I1" s="3" t="s">
         <v>24</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -3791,13 +3785,13 @@
         <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D2" t="s">
         <v>9</v>
       </c>
       <c r="F2" t="s">
-        <v>19</v>
+        <v>439</v>
       </c>
       <c r="G2" t="s">
         <v>10</v>
@@ -3808,35 +3802,35 @@
         <v>12</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C3" t="s">
         <v>11</v>
       </c>
       <c r="D3" t="s">
-        <v>482</v>
+        <v>484</v>
       </c>
       <c r="F3" t="s">
-        <v>19</v>
+        <v>439</v>
       </c>
       <c r="G3" t="s">
         <v>10</v>
       </c>
       <c r="H3" t="s">
+        <v>78</v>
+      </c>
+      <c r="I3" t="s">
         <v>79</v>
-      </c>
-      <c r="I3" t="s">
-        <v>80</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="Q14" r:id="rId1" display="www.facebook.com" xr:uid="{00000000-0004-0000-1000-000000000000}"/>
-    <hyperlink ref="R14" r:id="rId2" display="www.linkedin.com" xr:uid="{00000000-0004-0000-1000-000001000000}"/>
-    <hyperlink ref="Q15" r:id="rId3" display="www.facebook.com" xr:uid="{00000000-0004-0000-1000-000002000000}"/>
-    <hyperlink ref="R15" r:id="rId4" display="www.linkedin.com" xr:uid="{00000000-0004-0000-1000-000003000000}"/>
-    <hyperlink ref="Q3" r:id="rId5" display="www.facebook.com" xr:uid="{00000000-0004-0000-1000-000004000000}"/>
-    <hyperlink ref="R3" r:id="rId6" display="www.linkedin.com" xr:uid="{00000000-0004-0000-1000-000005000000}"/>
+    <hyperlink ref="Q14" r:id="rId1" display="www.facebook.com"/>
+    <hyperlink ref="R14" r:id="rId2" display="www.linkedin.com"/>
+    <hyperlink ref="Q15" r:id="rId3" display="www.facebook.com"/>
+    <hyperlink ref="R15" r:id="rId4" display="www.linkedin.com"/>
+    <hyperlink ref="Q3" r:id="rId5" display="www.facebook.com"/>
+    <hyperlink ref="R3" r:id="rId6" display="www.linkedin.com"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId7"/>
@@ -3844,7 +3838,7 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3869,57 +3863,57 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="D1" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="C1" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>109</v>
-      </c>
       <c r="E1" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F1" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="I1" s="5" t="s">
         <v>126</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="H1" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="I1" s="5" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B2" t="s">
-        <v>483</v>
+        <v>442</v>
       </c>
       <c r="C2" t="s">
-        <v>484</v>
+        <v>443</v>
       </c>
       <c r="D2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="H2" t="s">
+        <v>115</v>
+      </c>
+      <c r="I2" t="s">
         <v>116</v>
-      </c>
-      <c r="I2" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3929,11 +3923,11 @@
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3952,19 +3946,19 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C1" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="D1" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="E1" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>120</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>121</v>
       </c>
       <c r="G1" s="5"/>
       <c r="H1" s="5"/>
@@ -3972,22 +3966,22 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B2" t="s">
-        <v>485</v>
+        <v>440</v>
       </c>
       <c r="C2" t="s">
-        <v>486</v>
+        <v>441</v>
       </c>
       <c r="D2" t="s">
+        <v>121</v>
+      </c>
+      <c r="E2" t="s">
         <v>122</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>123</v>
-      </c>
-      <c r="F2" t="s">
-        <v>124</v>
       </c>
     </row>
   </sheetData>
@@ -3997,7 +3991,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4023,86 +4017,86 @@
         <v>1</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E1" s="5" t="s">
+        <v>309</v>
+      </c>
+      <c r="F1" s="5" t="s">
         <v>310</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>311</v>
       </c>
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>247</v>
+      </c>
+      <c r="B2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" t="s">
         <v>248</v>
       </c>
-      <c r="B2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="E2" s="20" t="s">
+        <v>231</v>
+      </c>
+      <c r="F2" t="s">
+        <v>413</v>
+      </c>
+      <c r="X2" s="27" t="s">
         <v>249</v>
-      </c>
-      <c r="E2" s="20" t="s">
-        <v>232</v>
-      </c>
-      <c r="F2" t="s">
-        <v>423</v>
-      </c>
-      <c r="X2" s="27" t="s">
-        <v>250</v>
       </c>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>250</v>
+      </c>
+      <c r="B3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" t="s">
         <v>251</v>
       </c>
-      <c r="B3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C3" t="s">
-        <v>252</v>
-      </c>
       <c r="E3" s="20" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="F3" t="s">
-        <v>424</v>
+        <v>414</v>
       </c>
       <c r="X3" s="27"/>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>252</v>
+      </c>
+      <c r="B4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" t="s">
         <v>253</v>
       </c>
-      <c r="B4" t="s">
-        <v>34</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>254</v>
       </c>
-      <c r="D4" t="s">
-        <v>255</v>
-      </c>
       <c r="E4" s="20" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="X4" s="27"/>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>255</v>
+      </c>
+      <c r="B5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5" t="s">
         <v>256</v>
       </c>
-      <c r="B5" t="s">
-        <v>36</v>
-      </c>
-      <c r="C5" t="s">
-        <v>257</v>
-      </c>
       <c r="E5" s="20" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="F5">
         <v>5000000</v>
@@ -4111,16 +4105,16 @@
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>257</v>
+      </c>
+      <c r="B6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C6" t="s">
         <v>258</v>
       </c>
-      <c r="B6" t="s">
-        <v>36</v>
-      </c>
-      <c r="C6" t="s">
-        <v>259</v>
-      </c>
       <c r="E6" s="20" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="X6" s="27"/>
     </row>
@@ -4133,11 +4127,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4157,10 +4151,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>2</v>
@@ -4172,197 +4166,197 @@
         <v>7</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B2" t="s">
-        <v>415</v>
+        <v>450</v>
       </c>
       <c r="C2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D2" t="s">
         <v>11</v>
       </c>
       <c r="E2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F2" t="s">
+        <v>83</v>
+      </c>
+      <c r="G2" t="s">
         <v>84</v>
       </c>
-      <c r="G2" t="s">
-        <v>85</v>
-      </c>
       <c r="H2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B3" t="s">
-        <v>416</v>
+        <v>451</v>
       </c>
       <c r="C3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D3" t="s">
         <v>11</v>
       </c>
       <c r="E3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G3" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="H3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B4" t="s">
-        <v>417</v>
+        <v>452</v>
       </c>
       <c r="C4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D4" t="s">
         <v>11</v>
       </c>
       <c r="E4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G4" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="H4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B5" t="s">
-        <v>418</v>
+        <v>453</v>
       </c>
       <c r="C5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D5" t="s">
         <v>11</v>
       </c>
       <c r="E5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G5" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="H5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B6" t="s">
-        <v>419</v>
+        <v>454</v>
       </c>
       <c r="C6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D6" t="s">
         <v>11</v>
       </c>
       <c r="E6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G6" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="H6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B7" t="s">
-        <v>420</v>
+        <v>455</v>
       </c>
       <c r="C7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D7" t="s">
         <v>11</v>
       </c>
       <c r="E7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G7" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="H7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B8" t="s">
-        <v>421</v>
+        <v>456</v>
       </c>
       <c r="C8" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D8" t="s">
         <v>11</v>
       </c>
       <c r="E8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G8" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="H8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B9" t="s">
-        <v>422</v>
+        <v>457</v>
       </c>
       <c r="C9" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D9" t="s">
         <v>11</v>
       </c>
       <c r="E9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G9" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="H9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -4371,7 +4365,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AM11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4437,220 +4431,220 @@
         <v>4</v>
       </c>
       <c r="F1" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="N1" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="O1" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="P1" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="Q1" s="5" t="s">
+        <v>367</v>
+      </c>
+      <c r="R1" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="G1" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="H1" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="I1" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="J1" s="5" t="s">
-        <v>140</v>
-      </c>
-      <c r="K1" s="5" t="s">
-        <v>141</v>
-      </c>
-      <c r="L1" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="M1" s="5" t="s">
-        <v>143</v>
-      </c>
-      <c r="N1" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="O1" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="P1" s="5" t="s">
-        <v>144</v>
-      </c>
-      <c r="Q1" s="5" t="s">
+      <c r="S1" s="5" t="s">
         <v>368</v>
       </c>
-      <c r="R1" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="S1" s="5" t="s">
+      <c r="T1" s="5" t="s">
+        <v>356</v>
+      </c>
+      <c r="U1" s="5" t="s">
         <v>369</v>
       </c>
-      <c r="T1" s="5" t="s">
-        <v>357</v>
-      </c>
-      <c r="U1" s="5" t="s">
-        <v>370</v>
-      </c>
       <c r="V1" s="5" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="AL1" s="3"/>
     </row>
     <row r="2" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B2" t="s">
         <v>11</v>
       </c>
       <c r="C2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E2" t="s">
-        <v>432</v>
+        <v>446</v>
       </c>
     </row>
     <row r="3" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B3" t="s">
         <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E3" t="s">
-        <v>433</v>
+        <v>447</v>
       </c>
     </row>
     <row r="4" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B4" t="s">
         <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E4" t="s">
-        <v>434</v>
+        <v>448</v>
       </c>
     </row>
     <row r="5" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B5" t="s">
         <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B6" t="s">
         <v>11</v>
       </c>
       <c r="C6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E6" t="s">
-        <v>430</v>
+        <v>444</v>
       </c>
     </row>
     <row r="7" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B7" t="s">
+        <v>64</v>
+      </c>
+      <c r="C7" t="s">
         <v>65</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
+        <v>47</v>
+      </c>
+      <c r="E7" t="s">
+        <v>445</v>
+      </c>
+      <c r="L7" t="s">
         <v>66</v>
       </c>
-      <c r="D7" t="s">
-        <v>48</v>
-      </c>
-      <c r="E7" t="s">
-        <v>431</v>
-      </c>
-      <c r="L7" t="s">
+      <c r="M7" t="s">
         <v>67</v>
       </c>
-      <c r="M7" t="s">
-        <v>68</v>
-      </c>
       <c r="N7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="O7">
         <v>654927</v>
       </c>
       <c r="P7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="B8" t="s">
+        <v>346</v>
+      </c>
+      <c r="C8" t="s">
         <v>347</v>
       </c>
-      <c r="C8" t="s">
-        <v>348</v>
-      </c>
       <c r="D8" t="s">
+        <v>315</v>
+      </c>
+      <c r="E8" t="s">
+        <v>477</v>
+      </c>
+      <c r="F8" t="s">
         <v>316</v>
       </c>
-      <c r="E8" t="s">
-        <v>449</v>
-      </c>
-      <c r="F8" t="s">
-        <v>317</v>
-      </c>
       <c r="G8" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="H8" t="s">
+        <v>42</v>
+      </c>
+      <c r="I8" t="s">
         <v>43</v>
-      </c>
-      <c r="I8" t="s">
-        <v>44</v>
       </c>
       <c r="J8">
         <v>281001</v>
       </c>
       <c r="K8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="L8" t="s">
+        <v>321</v>
+      </c>
+      <c r="M8" t="s">
         <v>322</v>
       </c>
-      <c r="M8" t="s">
+      <c r="N8" t="s">
         <v>323</v>
-      </c>
-      <c r="N8" t="s">
-        <v>324</v>
       </c>
       <c r="O8">
         <v>200300</v>
       </c>
       <c r="P8" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="Q8">
         <v>2121212121</v>
@@ -4662,7 +4656,7 @@
         <v>4141414141</v>
       </c>
       <c r="T8" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="U8">
         <v>5151515151</v>
@@ -4672,49 +4666,49 @@
     </row>
     <row r="9" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B9" t="s">
+        <v>346</v>
+      </c>
+      <c r="C9" t="s">
         <v>347</v>
       </c>
-      <c r="C9" t="s">
-        <v>348</v>
-      </c>
       <c r="D9" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="F9" t="s">
+        <v>325</v>
+      </c>
+      <c r="G9" t="s">
         <v>326</v>
       </c>
-      <c r="G9" t="s">
+      <c r="H9" t="s">
         <v>327</v>
       </c>
-      <c r="H9" t="s">
-        <v>328</v>
-      </c>
       <c r="I9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J9">
         <v>201301</v>
       </c>
       <c r="K9" t="s">
+        <v>328</v>
+      </c>
+      <c r="L9" t="s">
+        <v>371</v>
+      </c>
+      <c r="M9" t="s">
         <v>329</v>
       </c>
-      <c r="L9" t="s">
-        <v>372</v>
-      </c>
-      <c r="M9" t="s">
-        <v>330</v>
-      </c>
       <c r="N9" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="O9">
         <v>10016</v>
       </c>
       <c r="P9" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="Q9">
         <v>98765429</v>
@@ -4726,7 +4720,7 @@
         <v>4141414141</v>
       </c>
       <c r="T9" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="U9">
         <v>5151515151</v>
@@ -4736,49 +4730,49 @@
     </row>
     <row r="10" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B10" t="s">
+        <v>346</v>
+      </c>
+      <c r="C10" t="s">
         <v>347</v>
       </c>
-      <c r="C10" t="s">
-        <v>348</v>
-      </c>
       <c r="D10" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="F10" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="G10" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="H10" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="I10" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="J10">
         <v>500700</v>
       </c>
       <c r="K10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="L10" t="s">
+        <v>332</v>
+      </c>
+      <c r="M10" t="s">
         <v>333</v>
       </c>
-      <c r="M10" t="s">
-        <v>334</v>
-      </c>
       <c r="N10" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="O10">
         <v>2834</v>
       </c>
       <c r="P10" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="Q10">
         <v>1629539588</v>
@@ -4790,7 +4784,7 @@
         <v>4141414141</v>
       </c>
       <c r="T10" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="U10">
         <v>5151515151</v>
@@ -4800,52 +4794,52 @@
     </row>
     <row r="11" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B11" t="s">
+        <v>349</v>
+      </c>
+      <c r="C11" t="s">
         <v>350</v>
       </c>
-      <c r="C11" t="s">
-        <v>351</v>
-      </c>
       <c r="D11" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E11" t="s">
-        <v>450</v>
+        <v>478</v>
       </c>
       <c r="F11" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="G11" t="s">
+        <v>340</v>
+      </c>
+      <c r="H11" t="s">
+        <v>388</v>
+      </c>
+      <c r="I11" t="s">
         <v>341</v>
-      </c>
-      <c r="H11" t="s">
-        <v>389</v>
-      </c>
-      <c r="I11" t="s">
-        <v>342</v>
       </c>
       <c r="J11">
         <v>560003</v>
       </c>
       <c r="K11" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="L11" t="s">
+        <v>340</v>
+      </c>
+      <c r="M11" t="s">
+        <v>388</v>
+      </c>
+      <c r="N11" t="s">
         <v>341</v>
-      </c>
-      <c r="M11" t="s">
-        <v>389</v>
-      </c>
-      <c r="N11" t="s">
-        <v>342</v>
       </c>
       <c r="O11">
         <v>560003</v>
       </c>
       <c r="P11" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="Q11">
         <v>9999999999</v>
@@ -4857,13 +4851,13 @@
         <v>9955875125</v>
       </c>
       <c r="T11" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="U11">
         <v>9595956632</v>
       </c>
       <c r="V11" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="AJ11" s="6"/>
       <c r="AK11"/>
@@ -4876,7 +4870,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4908,100 +4902,100 @@
         <v>5</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F1" s="22" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H1" s="9" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C2" t="s">
         <v>72</v>
       </c>
-      <c r="C2" t="s">
-        <v>73</v>
-      </c>
       <c r="D2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E2">
         <v>100</v>
       </c>
       <c r="F2" t="s">
-        <v>441</v>
+        <v>466</v>
       </c>
       <c r="G2">
         <v>2019</v>
       </c>
       <c r="H2" t="s">
-        <v>414</v>
+        <v>449</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E3">
         <v>100</v>
       </c>
       <c r="F3" s="24" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="G3">
         <v>2020</v>
       </c>
       <c r="H3" t="s">
-        <v>414</v>
+        <v>449</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E4">
         <v>100</v>
       </c>
       <c r="F4" t="s">
-        <v>444</v>
+        <v>471</v>
       </c>
       <c r="G4">
         <v>2021</v>
       </c>
       <c r="H4" t="s">
-        <v>414</v>
+        <v>449</v>
       </c>
     </row>
   </sheetData>
@@ -5011,12 +5005,12 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F2" sqref="F2"/>
+      <selection pane="bottomLeft" activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5035,148 +5029,148 @@
         <v>0</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C1" s="5" t="s">
         <v>5</v>
       </c>
       <c r="D1" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E1" s="8" t="s">
         <v>214</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="F1" s="5" t="s">
         <v>215</v>
       </c>
-      <c r="F1" s="5" t="s">
-        <v>216</v>
-      </c>
       <c r="G1" s="5" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>216</v>
+      </c>
+      <c r="B2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E2" t="s">
         <v>217</v>
       </c>
-      <c r="B2" t="s">
-        <v>83</v>
-      </c>
-      <c r="C2" t="s">
-        <v>72</v>
-      </c>
-      <c r="D2" t="s">
-        <v>34</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>218</v>
-      </c>
-      <c r="F2" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>219</v>
+      </c>
+      <c r="B3" t="s">
+        <v>85</v>
+      </c>
+      <c r="C3" t="s">
+        <v>73</v>
+      </c>
+      <c r="D3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E3" t="s">
+        <v>217</v>
+      </c>
+      <c r="F3" t="s">
         <v>220</v>
-      </c>
-      <c r="B3" t="s">
-        <v>86</v>
-      </c>
-      <c r="C3" t="s">
-        <v>74</v>
-      </c>
-      <c r="D3" t="s">
-        <v>36</v>
-      </c>
-      <c r="E3" t="s">
-        <v>218</v>
-      </c>
-      <c r="F3" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>229</v>
+      </c>
+      <c r="B4" t="s">
         <v>230</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
+        <v>73</v>
+      </c>
+      <c r="D4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E4" t="s">
+        <v>217</v>
+      </c>
+      <c r="F4" t="s">
         <v>231</v>
       </c>
-      <c r="C4" t="s">
-        <v>74</v>
-      </c>
-      <c r="D4" t="s">
-        <v>34</v>
-      </c>
-      <c r="E4" t="s">
-        <v>218</v>
-      </c>
-      <c r="F4" t="s">
-        <v>232</v>
-      </c>
       <c r="G4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E5" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="F5" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="G5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F6" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="G6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B7" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F7" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="G7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -5185,7 +5179,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5203,31 +5197,31 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -5236,7 +5230,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5268,148 +5262,148 @@
         <v>0</v>
       </c>
       <c r="B1" s="11" t="s">
+        <v>170</v>
+      </c>
+      <c r="C1" s="11" t="s">
         <v>171</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="D1" s="11" t="s">
+        <v>177</v>
+      </c>
+      <c r="E1" s="11" t="s">
         <v>172</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="F1" s="11" t="s">
+        <v>173</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>150</v>
+      </c>
+      <c r="H1" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="I1" s="11" t="s">
+        <v>174</v>
+      </c>
+      <c r="J1" s="11" t="s">
+        <v>175</v>
+      </c>
+      <c r="K1" s="11" t="s">
+        <v>176</v>
+      </c>
+      <c r="L1" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="M1" s="11" t="s">
+        <v>167</v>
+      </c>
+      <c r="N1" s="11" t="s">
+        <v>168</v>
+      </c>
+      <c r="O1" s="11" t="s">
         <v>178</v>
       </c>
-      <c r="E1" s="11" t="s">
-        <v>173</v>
-      </c>
-      <c r="F1" s="11" t="s">
-        <v>174</v>
-      </c>
-      <c r="G1" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="H1" s="11" t="s">
-        <v>152</v>
-      </c>
-      <c r="I1" s="11" t="s">
-        <v>175</v>
-      </c>
-      <c r="J1" s="11" t="s">
-        <v>176</v>
-      </c>
-      <c r="K1" s="11" t="s">
-        <v>177</v>
-      </c>
-      <c r="L1" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="M1" s="11" t="s">
-        <v>168</v>
-      </c>
-      <c r="N1" s="11" t="s">
-        <v>169</v>
-      </c>
-      <c r="O1" s="11" t="s">
+      <c r="P1" s="11" t="s">
         <v>179</v>
-      </c>
-      <c r="P1" s="11" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>152</v>
+      </c>
+      <c r="B2" t="s">
+        <v>474</v>
+      </c>
+      <c r="C2" t="s">
         <v>153</v>
       </c>
-      <c r="B2" t="s">
-        <v>446</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>154</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>155</v>
-      </c>
-      <c r="E2" t="s">
-        <v>156</v>
       </c>
       <c r="F2">
         <v>0</v>
       </c>
       <c r="G2" t="s">
+        <v>155</v>
+      </c>
+      <c r="H2" t="s">
         <v>156</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
+        <v>33</v>
+      </c>
+      <c r="J2" t="s">
         <v>157</v>
       </c>
-      <c r="I2" t="s">
-        <v>34</v>
-      </c>
-      <c r="J2" t="s">
-        <v>158</v>
-      </c>
       <c r="O2" t="s">
+        <v>180</v>
+      </c>
+      <c r="P2" t="s">
         <v>181</v>
-      </c>
-      <c r="P2" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>158</v>
+      </c>
+      <c r="B3" t="s">
+        <v>475</v>
+      </c>
+      <c r="C3" t="s">
         <v>159</v>
-      </c>
-      <c r="B3" t="s">
-        <v>447</v>
-      </c>
-      <c r="C3" t="s">
-        <v>160</v>
       </c>
       <c r="F3">
         <v>0</v>
       </c>
       <c r="G3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H3" t="s">
+        <v>160</v>
+      </c>
+      <c r="I3" t="s">
         <v>161</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>162</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>163</v>
-      </c>
-      <c r="K3" t="s">
-        <v>164</v>
       </c>
       <c r="L3">
         <v>25</v>
       </c>
       <c r="M3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="N3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>164</v>
+      </c>
+      <c r="B4" t="s">
+        <v>476</v>
+      </c>
+      <c r="C4" t="s">
         <v>165</v>
       </c>
-      <c r="B4" t="s">
-        <v>448</v>
-      </c>
-      <c r="C4" t="s">
-        <v>166</v>
-      </c>
       <c r="G4" t="s">
+        <v>155</v>
+      </c>
+      <c r="H4" t="s">
         <v>156</v>
       </c>
-      <c r="H4" t="s">
-        <v>157</v>
-      </c>
       <c r="I4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -5419,7 +5413,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5446,63 +5440,63 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>183</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>184</v>
       </c>
-      <c r="F1" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>185</v>
       </c>
-      <c r="H1" s="3" t="s">
-        <v>186</v>
-      </c>
       <c r="I1" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="L1" s="4" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>186</v>
+      </c>
+      <c r="B2" t="s">
         <v>187</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>188</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>189</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>190</v>
       </c>
-      <c r="E2" t="s">
-        <v>191</v>
-      </c>
       <c r="F2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G2">
         <v>201300</v>
       </c>
       <c r="H2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I2">
         <v>243634535</v>
@@ -5511,36 +5505,36 @@
         <v>8867765</v>
       </c>
       <c r="K2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="L2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>192</v>
+      </c>
+      <c r="B3" t="s">
         <v>193</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>194</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>195</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
+        <v>43</v>
+      </c>
+      <c r="F3" t="s">
         <v>196</v>
-      </c>
-      <c r="E3" t="s">
-        <v>44</v>
-      </c>
-      <c r="F3" t="s">
-        <v>197</v>
       </c>
       <c r="G3">
         <v>400523</v>
       </c>
       <c r="H3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I3">
         <v>599546546</v>
@@ -5549,36 +5543,36 @@
         <v>1084566</v>
       </c>
       <c r="K3" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="L3" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>198</v>
+      </c>
+      <c r="B4" t="s">
         <v>199</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>200</v>
       </c>
-      <c r="C4" t="s">
-        <v>201</v>
-      </c>
       <c r="D4" t="s">
+        <v>189</v>
+      </c>
+      <c r="E4" t="s">
         <v>190</v>
       </c>
-      <c r="E4" t="s">
-        <v>191</v>
-      </c>
       <c r="F4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G4">
         <v>500900</v>
       </c>
       <c r="H4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I4">
         <v>745465656</v>
@@ -5587,7 +5581,7 @@
         <v>45654656</v>
       </c>
       <c r="K4" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
   </sheetData>

</xml_diff>